<commit_message>
abstract: Lexical flexibility: Expanding the empirical coverage
</commit_message>
<xml_diff>
--- a/thesis/progress.xlsx
+++ b/thesis/progress.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f7cf2c9d3dc7fdc6/Dissertation/thesis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="165" documentId="8_{8233B9E9-5E46-417E-8631-6A32EFB57DCE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{0C78AC2A-6C58-4F28-A7B7-A7A22E4E2C1B}"/>
+  <xr:revisionPtr revIDLastSave="173" documentId="8_{8233B9E9-5E46-417E-8631-6A32EFB57DCE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{B056D31E-F26A-41BA-BBE1-53CC5FCD5CAA}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{90EBE93A-7825-427E-BCBE-4711C8076B47}"/>
   </bookViews>
@@ -311,10 +311,10 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>writing!$A$2:$A$7</c:f>
+              <c:f>writing!$A$2:$A$8</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>44130</c:v>
                 </c:pt>
@@ -332,16 +332,19 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>44135</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>44136</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>writing!$K$2:$K$7</c:f>
+              <c:f>writing!$K$2:$K$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>1360</c:v>
                 </c:pt>
@@ -359,6 +362,9 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>1489</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>621</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -470,10 +476,10 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>writing!$A$2:$A$7</c:f>
+              <c:f>writing!$A$2:$A$8</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>44130</c:v>
                 </c:pt>
@@ -491,16 +497,19 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>44135</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>44136</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>writing!$J$2:$J$7</c:f>
+              <c:f>writing!$J$2:$J$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>2225</c:v>
                 </c:pt>
@@ -517,6 +526,9 @@
                   <c:v>6044</c:v>
                 </c:pt>
                 <c:pt idx="5">
+                  <c:v>7533</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>7533</c:v>
                 </c:pt>
               </c:numCache>
@@ -1486,8 +1498,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{65BC4CFE-CBD1-4A0C-ACAB-8E0C8A33A81F}" name="Table1" displayName="Table1" ref="A1:K7" totalsRowShown="0" headerRowDxfId="1">
-  <autoFilter ref="A1:K7" xr:uid="{5C2EF26B-8F7C-40DC-90B6-805AC60B672A}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{65BC4CFE-CBD1-4A0C-ACAB-8E0C8A33A81F}" name="Table1" displayName="Table1" ref="A1:K8" totalsRowShown="0" headerRowDxfId="1">
+  <autoFilter ref="A1:K8" xr:uid="{5C2EF26B-8F7C-40DC-90B6-805AC60B672A}"/>
   <tableColumns count="11">
     <tableColumn id="1" xr3:uid="{BEA871B4-EEE2-4F93-9DBC-4AFC40E06E5F}" name="Date" dataDxfId="0"/>
     <tableColumn id="2" xr3:uid="{3081B1F4-64BE-4187-A6E1-DC702177CD85}" name="Abstract"/>
@@ -1821,10 +1833,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F901F93A-6EBC-444E-BB8F-D0008D03E2AA}">
-  <dimension ref="A1:K7"/>
+  <dimension ref="A1:K8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1906,7 +1918,7 @@
         <v>0</v>
       </c>
       <c r="J2">
-        <f>SUM(B2:I2)</f>
+        <f t="shared" ref="J2:J7" si="0">SUM(B2:I2)</f>
         <v>2225</v>
       </c>
       <c r="K2">
@@ -1942,7 +1954,7 @@
         <v>0</v>
       </c>
       <c r="J3">
-        <f>SUM(B3:I3)</f>
+        <f t="shared" si="0"/>
         <v>3239</v>
       </c>
       <c r="K3">
@@ -1979,7 +1991,7 @@
         <v>0</v>
       </c>
       <c r="J4">
-        <f>SUM(B4:I4)</f>
+        <f t="shared" si="0"/>
         <v>4040</v>
       </c>
       <c r="K4">
@@ -2016,7 +2028,7 @@
         <v>0</v>
       </c>
       <c r="J5">
-        <f>SUM(B5:I5)</f>
+        <f t="shared" si="0"/>
         <v>5281</v>
       </c>
       <c r="K5">
@@ -2053,7 +2065,7 @@
         <v>0</v>
       </c>
       <c r="J6">
-        <f>SUM(B6:I6)</f>
+        <f t="shared" si="0"/>
         <v>6044</v>
       </c>
       <c r="K6">
@@ -2090,20 +2102,56 @@
         <v>5</v>
       </c>
       <c r="J7">
-        <f>SUM(B7:I7)</f>
+        <f t="shared" si="0"/>
         <v>7533</v>
       </c>
       <c r="K7">
         <f>J7-J6</f>
         <v>1489</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A8" s="1">
+        <v>44136</v>
+      </c>
+      <c r="B8">
+        <v>239</v>
+      </c>
+      <c r="C8">
+        <v>87</v>
+      </c>
+      <c r="D8">
+        <v>528</v>
+      </c>
+      <c r="E8">
+        <v>6658</v>
+      </c>
+      <c r="F8">
+        <v>5</v>
+      </c>
+      <c r="G8">
+        <v>6</v>
+      </c>
+      <c r="H8">
+        <v>5</v>
+      </c>
+      <c r="I8">
+        <v>5</v>
+      </c>
+      <c r="J8">
+        <f>SUM(B8:I8)</f>
+        <v>7533</v>
+      </c>
+      <c r="K8">
+        <v>621</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="J2:J7" formulaRange="1"/>
-    <ignoredError sqref="K2" calculatedColumn="1"/>
+    <ignoredError sqref="J2:J8" formulaRange="1"/>
+    <ignoredError sqref="K2 K8" calculatedColumn="1"/>
   </ignoredErrors>
   <tableParts count="1">
     <tablePart r:id="rId2"/>

</xml_diff>

<commit_message>
finish draft of Introduction
</commit_message>
<xml_diff>
--- a/thesis/progress.xlsx
+++ b/thesis/progress.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f7cf2c9d3dc7fdc6/Dissertation/thesis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="179" documentId="8_{8233B9E9-5E46-417E-8631-6A32EFB57DCE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{EA6E347A-D688-43FA-A3F2-1A989AA6A322}"/>
+  <xr:revisionPtr revIDLastSave="184" documentId="8_{8233B9E9-5E46-417E-8631-6A32EFB57DCE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{04495D7C-FA63-4364-B117-E75A85002285}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{90EBE93A-7825-427E-BCBE-4711C8076B47}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{90EBE93A-7825-427E-BCBE-4711C8076B47}"/>
   </bookViews>
   <sheets>
     <sheet name="dashboard" sheetId="3" r:id="rId1"/>
@@ -311,10 +311,10 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>writing!$A$2:$A$9</c:f>
+              <c:f>writing!$A$2:$A$10</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>44130</c:v>
                 </c:pt>
@@ -338,16 +338,19 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>44137</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>44138</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>writing!$K$2:$K$9</c:f>
+              <c:f>writing!$K$2:$K$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>1360</c:v>
                 </c:pt>
@@ -371,6 +374,9 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>811</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>210</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -482,10 +488,10 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>writing!$A$2:$A$9</c:f>
+              <c:f>writing!$A$2:$A$10</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>44130</c:v>
                 </c:pt>
@@ -509,16 +515,19 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>44137</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>44138</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>writing!$J$2:$J$9</c:f>
+              <c:f>writing!$J$2:$J$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>2225</c:v>
                 </c:pt>
@@ -542,6 +551,9 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>8344</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8554</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1510,8 +1522,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{65BC4CFE-CBD1-4A0C-ACAB-8E0C8A33A81F}" name="Table1" displayName="Table1" ref="A1:K9" totalsRowShown="0" headerRowDxfId="1">
-  <autoFilter ref="A1:K9" xr:uid="{5C2EF26B-8F7C-40DC-90B6-805AC60B672A}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{65BC4CFE-CBD1-4A0C-ACAB-8E0C8A33A81F}" name="Table1" displayName="Table1" ref="A1:K10" totalsRowShown="0" headerRowDxfId="1">
+  <autoFilter ref="A1:K10" xr:uid="{5C2EF26B-8F7C-40DC-90B6-805AC60B672A}"/>
   <tableColumns count="11">
     <tableColumn id="1" xr3:uid="{BEA871B4-EEE2-4F93-9DBC-4AFC40E06E5F}" name="Date" dataDxfId="0"/>
     <tableColumn id="2" xr3:uid="{3081B1F4-64BE-4187-A6E1-DC702177CD85}" name="Abstract"/>
@@ -1832,7 +1844,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CEB7023-1E9A-48AE-8417-31A8A140F136}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="T13" sqref="T13"/>
     </sheetView>
   </sheetViews>
@@ -1845,10 +1857,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F901F93A-6EBC-444E-BB8F-D0008D03E2AA}">
-  <dimension ref="A1:K9"/>
+  <dimension ref="A1:K10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2195,11 +2207,48 @@
         <v>811</v>
       </c>
     </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A10" s="1">
+        <v>44138</v>
+      </c>
+      <c r="B10">
+        <v>239</v>
+      </c>
+      <c r="C10">
+        <v>87</v>
+      </c>
+      <c r="D10">
+        <v>528</v>
+      </c>
+      <c r="E10">
+        <v>7638</v>
+      </c>
+      <c r="F10">
+        <v>46</v>
+      </c>
+      <c r="G10">
+        <v>6</v>
+      </c>
+      <c r="H10">
+        <v>5</v>
+      </c>
+      <c r="I10">
+        <v>5</v>
+      </c>
+      <c r="J10">
+        <f>SUM(B10:I10)</f>
+        <v>8554</v>
+      </c>
+      <c r="K10">
+        <f>J10-J9</f>
+        <v>210</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="J2:J9" formulaRange="1"/>
+    <ignoredError sqref="J2:J10" formulaRange="1"/>
     <ignoredError sqref="K2 K8" calculatedColumn="1"/>
   </ignoredErrors>
   <tableParts count="1">

</xml_diff>

<commit_message>
Chapter 1: revisions (v0.3.2)
</commit_message>
<xml_diff>
--- a/thesis/progress.xlsx
+++ b/thesis/progress.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f7cf2c9d3dc7fdc6/Dissertation/thesis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="205" documentId="8_{8233B9E9-5E46-417E-8631-6A32EFB57DCE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{9634BD7F-F19B-4E7F-8A55-9222A57316F7}"/>
+  <xr:revisionPtr revIDLastSave="213" documentId="8_{8233B9E9-5E46-417E-8631-6A32EFB57DCE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{6465B0AF-6C3F-4759-8BD2-C845926F2907}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{90EBE93A-7825-427E-BCBE-4711C8076B47}"/>
   </bookViews>
@@ -333,10 +333,10 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>writing!$A$2:$A$11</c:f>
+              <c:f>writing!$A$2:$A$12</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>44130</c:v>
                 </c:pt>
@@ -366,16 +366,19 @@
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>44139</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>44142</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>writing!$K$2:$K$11</c:f>
+              <c:f>writing!$K$2:$K$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>1360</c:v>
                 </c:pt>
@@ -405,6 +408,9 @@
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>56</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>75</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -516,10 +522,10 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>writing!$A$2:$A$11</c:f>
+              <c:f>writing!$A$2:$A$12</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>44130</c:v>
                 </c:pt>
@@ -549,16 +555,19 @@
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>44139</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>44142</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>writing!$J$2:$J$11</c:f>
+              <c:f>writing!$J$2:$J$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>2225</c:v>
                 </c:pt>
@@ -588,6 +597,9 @@
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>8524</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>8599</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1556,8 +1568,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{65BC4CFE-CBD1-4A0C-ACAB-8E0C8A33A81F}" name="Table1" displayName="Table1" ref="A1:K11" totalsRowShown="0" headerRowDxfId="1">
-  <autoFilter ref="A1:K11" xr:uid="{5C2EF26B-8F7C-40DC-90B6-805AC60B672A}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{65BC4CFE-CBD1-4A0C-ACAB-8E0C8A33A81F}" name="Table1" displayName="Table1" ref="A1:K12" totalsRowShown="0" headerRowDxfId="1">
+  <autoFilter ref="A1:K12" xr:uid="{5C2EF26B-8F7C-40DC-90B6-805AC60B672A}"/>
   <tableColumns count="11">
     <tableColumn id="1" xr3:uid="{BEA871B4-EEE2-4F93-9DBC-4AFC40E06E5F}" name="Date" dataDxfId="0"/>
     <tableColumn id="2" xr3:uid="{3081B1F4-64BE-4187-A6E1-DC702177CD85}" name="Abstract"/>
@@ -1891,10 +1903,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F901F93A-6EBC-444E-BB8F-D0008D03E2AA}">
-  <dimension ref="A1:K11"/>
+  <dimension ref="A1:K12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2315,11 +2327,48 @@
         <v>56</v>
       </c>
     </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A12" s="1">
+        <v>44142</v>
+      </c>
+      <c r="B12">
+        <v>239</v>
+      </c>
+      <c r="C12">
+        <v>87</v>
+      </c>
+      <c r="D12">
+        <v>547</v>
+      </c>
+      <c r="E12">
+        <v>7413</v>
+      </c>
+      <c r="F12">
+        <v>297</v>
+      </c>
+      <c r="G12">
+        <v>6</v>
+      </c>
+      <c r="H12">
+        <v>5</v>
+      </c>
+      <c r="I12">
+        <v>5</v>
+      </c>
+      <c r="J12">
+        <f>SUM(B12:I12)</f>
+        <v>8599</v>
+      </c>
+      <c r="K12">
+        <f>J12-J11</f>
+        <v>75</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="J2:J11" formulaRange="1"/>
+    <ignoredError sqref="J2:J12" formulaRange="1"/>
     <ignoredError sqref="K2 K8" calculatedColumn="1"/>
     <ignoredError sqref="K11" formulaRange="1" calculatedColumn="1"/>
   </ignoredErrors>

</xml_diff>

<commit_message>
update plots; create slides (#926)
</commit_message>
<xml_diff>
--- a/thesis/progress.xlsx
+++ b/thesis/progress.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f7cf2c9d3dc7fdc6/Dissertation/thesis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="222" documentId="8_{8233B9E9-5E46-417E-8631-6A32EFB57DCE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{D0924E07-EAD0-4B7A-AF4E-272106E2F367}"/>
+  <xr:revisionPtr revIDLastSave="226" documentId="8_{8233B9E9-5E46-417E-8631-6A32EFB57DCE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{670F7B08-B672-4022-9063-0423C8DA43BD}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" activeTab="1" xr2:uid="{90EBE93A-7825-427E-BCBE-4711C8076B47}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{90EBE93A-7825-427E-BCBE-4711C8076B47}"/>
   </bookViews>
   <sheets>
     <sheet name="dashboard" sheetId="3" r:id="rId1"/>
@@ -333,10 +333,10 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>writing!$A$2:$A$13</c:f>
+              <c:f>writing!$A$2:$A$14</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
                   <c:v>44130</c:v>
                 </c:pt>
@@ -372,16 +372,19 @@
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>44144</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>44146</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>writing!$K$2:$K$13</c:f>
+              <c:f>writing!$K$2:$K$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
                   <c:v>1360</c:v>
                 </c:pt>
@@ -417,6 +420,9 @@
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>511</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2671</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -528,10 +534,10 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>writing!$A$2:$A$13</c:f>
+              <c:f>writing!$A$2:$A$14</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
                   <c:v>44130</c:v>
                 </c:pt>
@@ -567,16 +573,19 @@
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>44144</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>44146</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>writing!$J$2:$J$13</c:f>
+              <c:f>writing!$J$2:$J$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
                   <c:v>2225</c:v>
                 </c:pt>
@@ -611,6 +620,9 @@
                   <c:v>8599</c:v>
                 </c:pt>
                 <c:pt idx="11">
+                  <c:v>9110</c:v>
+                </c:pt>
+                <c:pt idx="12">
                   <c:v>9110</c:v>
                 </c:pt>
               </c:numCache>
@@ -1580,8 +1592,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{65BC4CFE-CBD1-4A0C-ACAB-8E0C8A33A81F}" name="Table1" displayName="Table1" ref="A1:K13" totalsRowShown="0" headerRowDxfId="1">
-  <autoFilter ref="A1:K13" xr:uid="{5C2EF26B-8F7C-40DC-90B6-805AC60B672A}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{65BC4CFE-CBD1-4A0C-ACAB-8E0C8A33A81F}" name="Table1" displayName="Table1" ref="A1:K14" totalsRowShown="0" headerRowDxfId="1">
+  <autoFilter ref="A1:K14" xr:uid="{5C2EF26B-8F7C-40DC-90B6-805AC60B672A}"/>
   <tableColumns count="11">
     <tableColumn id="1" xr3:uid="{BEA871B4-EEE2-4F93-9DBC-4AFC40E06E5F}" name="Date" dataDxfId="0"/>
     <tableColumn id="2" xr3:uid="{3081B1F4-64BE-4187-A6E1-DC702177CD85}" name="Abstract"/>
@@ -1902,7 +1914,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CEB7023-1E9A-48AE-8417-31A8A140F136}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="T13" sqref="T13"/>
     </sheetView>
   </sheetViews>
@@ -1915,10 +1927,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F901F93A-6EBC-444E-BB8F-D0008D03E2AA}">
-  <dimension ref="A1:K13"/>
+  <dimension ref="A1:K14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2221,7 +2233,7 @@
         <v>5</v>
       </c>
       <c r="J8">
-        <f>SUM(B8:I8)</f>
+        <f t="shared" ref="J8:J13" si="1">SUM(B8:I8)</f>
         <v>7533</v>
       </c>
       <c r="K8">
@@ -2257,7 +2269,7 @@
         <v>5</v>
       </c>
       <c r="J9">
-        <f>SUM(B9:I9)</f>
+        <f t="shared" si="1"/>
         <v>8344</v>
       </c>
       <c r="K9">
@@ -2294,7 +2306,7 @@
         <v>5</v>
       </c>
       <c r="J10">
-        <f>SUM(B10:I10)</f>
+        <f t="shared" si="1"/>
         <v>8554</v>
       </c>
       <c r="K10">
@@ -2331,7 +2343,7 @@
         <v>5</v>
       </c>
       <c r="J11">
-        <f>SUM(B11:I11)</f>
+        <f t="shared" si="1"/>
         <v>8524</v>
       </c>
       <c r="K11" cm="1">
@@ -2368,7 +2380,7 @@
         <v>5</v>
       </c>
       <c r="J12">
-        <f>SUM(B12:I12)</f>
+        <f t="shared" si="1"/>
         <v>8599</v>
       </c>
       <c r="K12">
@@ -2405,20 +2417,56 @@
         <v>186</v>
       </c>
       <c r="J13">
-        <f>SUM(B13:I13)</f>
+        <f t="shared" si="1"/>
         <v>9110</v>
       </c>
       <c r="K13">
         <f>J13-J12</f>
         <v>511</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A14" s="1">
+        <v>44146</v>
+      </c>
+      <c r="B14">
+        <v>239</v>
+      </c>
+      <c r="C14">
+        <v>87</v>
+      </c>
+      <c r="D14">
+        <v>547</v>
+      </c>
+      <c r="E14">
+        <v>7413</v>
+      </c>
+      <c r="F14">
+        <v>401</v>
+      </c>
+      <c r="G14">
+        <v>120</v>
+      </c>
+      <c r="H14">
+        <v>117</v>
+      </c>
+      <c r="I14">
+        <v>186</v>
+      </c>
+      <c r="J14">
+        <f>SUM(B14:I14)</f>
+        <v>9110</v>
+      </c>
+      <c r="K14">
+        <v>2671</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="J2:J13" formulaRange="1"/>
-    <ignoredError sqref="K2 K8" calculatedColumn="1"/>
+    <ignoredError sqref="J2:J14" formulaRange="1"/>
+    <ignoredError sqref="K2 K8 K14" calculatedColumn="1"/>
     <ignoredError sqref="K11" formulaRange="1" calculatedColumn="1"/>
   </ignoredErrors>
   <tableParts count="1">

</xml_diff>

<commit_message>
Section 2.2: Traditional approaches in progress
</commit_message>
<xml_diff>
--- a/thesis/progress.xlsx
+++ b/thesis/progress.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f7cf2c9d3dc7fdc6/Dissertation/thesis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="235" documentId="8_{8233B9E9-5E46-417E-8631-6A32EFB57DCE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{CE209FE3-A1E1-4FAF-AEC3-FE4A073046ED}"/>
+  <xr:revisionPtr revIDLastSave="236" documentId="8_{8233B9E9-5E46-417E-8631-6A32EFB57DCE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{333D3BAD-AA71-407D-AEAF-D5722F016E44}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" activeTab="1" xr2:uid="{90EBE93A-7825-427E-BCBE-4711C8076B47}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{90EBE93A-7825-427E-BCBE-4711C8076B47}"/>
   </bookViews>
   <sheets>
     <sheet name="dashboard" sheetId="3" r:id="rId1"/>
@@ -428,7 +428,7 @@
                   <c:v>2671</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>176</c:v>
+                  <c:v>577</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1926,7 +1926,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CEB7023-1E9A-48AE-8417-31A8A140F136}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="T13" sqref="T13"/>
     </sheetView>
   </sheetViews>
@@ -1941,8 +1941,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F901F93A-6EBC-444E-BB8F-D0008D03E2AA}">
   <dimension ref="A1:K15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2506,16 +2506,15 @@
         <v>9286</v>
       </c>
       <c r="K15">
-        <f>J15-J14</f>
-        <v>176</v>
+        <v>577</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="J2:J14" formulaRange="1"/>
-    <ignoredError sqref="K2 K8 K14" calculatedColumn="1"/>
+    <ignoredError sqref="J2:J15" formulaRange="1"/>
+    <ignoredError sqref="K2 K8 K14:K15" calculatedColumn="1"/>
     <ignoredError sqref="K11" formulaRange="1" calculatedColumn="1"/>
   </ignoredErrors>
   <tableParts count="1">

</xml_diff>

<commit_message>
Section 2.3.1.4: Precategoriality / Acategoriality
</commit_message>
<xml_diff>
--- a/thesis/progress.xlsx
+++ b/thesis/progress.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f7cf2c9d3dc7fdc6/Dissertation/thesis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="286" documentId="8_{8233B9E9-5E46-417E-8631-6A32EFB57DCE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{580A1A01-A29A-41AC-8FB1-C94E97B7ADCC}"/>
+  <xr:revisionPtr revIDLastSave="318" documentId="8_{8233B9E9-5E46-417E-8631-6A32EFB57DCE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{ADCB6214-978D-46CB-9DC1-220AAAF39DB3}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{90EBE93A-7825-427E-BCBE-4711C8076B47}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" activeTab="1" xr2:uid="{90EBE93A-7825-427E-BCBE-4711C8076B47}"/>
   </bookViews>
   <sheets>
     <sheet name="dashboard" sheetId="3" r:id="rId1"/>
     <sheet name="writing" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029" calcCompleted="0"/>
+  <calcPr calcId="191028" calcCompleted="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -333,10 +333,10 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>writing!$A$2:$A$21</c:f>
+              <c:f>writing!$A$2:$A$24</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="20"/>
+                <c:ptCount val="23"/>
                 <c:pt idx="0">
                   <c:v>44130</c:v>
                 </c:pt>
@@ -396,16 +396,25 @@
                 </c:pt>
                 <c:pt idx="19">
                   <c:v>44154</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>44155</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>44156</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>44157</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>writing!$K$2:$K$21</c:f>
+              <c:f>writing!$K$2:$K$24</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="20"/>
+                <c:ptCount val="23"/>
                 <c:pt idx="0">
                   <c:v>1360</c:v>
                 </c:pt>
@@ -465,13 +474,22 @@
                 </c:pt>
                 <c:pt idx="19">
                   <c:v>56</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1136</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>679</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>467</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-43CA-48CC-BAB2-BC0740F4C54B}"/>
+              <c16:uniqueId val="{00000000-7415-4A85-8004-99D6E505098C}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -576,10 +594,10 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>writing!$A$2:$A$21</c:f>
+              <c:f>writing!$A$2:$A$24</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="20"/>
+                <c:ptCount val="23"/>
                 <c:pt idx="0">
                   <c:v>44130</c:v>
                 </c:pt>
@@ -639,16 +657,25 @@
                 </c:pt>
                 <c:pt idx="19">
                   <c:v>44154</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>44155</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>44156</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>44157</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>writing!$J$2:$J$21</c:f>
+              <c:f>writing!$J$2:$J$24</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="20"/>
+                <c:ptCount val="23"/>
                 <c:pt idx="0">
                   <c:v>2225</c:v>
                 </c:pt>
@@ -708,6 +735,15 @@
                 </c:pt>
                 <c:pt idx="19">
                   <c:v>12014</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>13150</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>13829</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>14296</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -715,7 +751,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-43CA-48CC-BAB2-BC0740F4C54B}"/>
+              <c16:uniqueId val="{00000001-7415-4A85-8004-99D6E505098C}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1645,14 +1681,14 @@
       <xdr:col>17</xdr:col>
       <xdr:colOff>195262</xdr:colOff>
       <xdr:row>27</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1">
+        <xdr:cNvPr id="3" name="Chart 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BC058E7F-7E39-412B-87BB-BD9ABB4BB559}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F2688EB1-1F21-4955-9B3B-F35A81E6A042}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1676,8 +1712,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{65BC4CFE-CBD1-4A0C-ACAB-8E0C8A33A81F}" name="Table1" displayName="Table1" ref="A1:K21" totalsRowShown="0" headerRowDxfId="1">
-  <autoFilter ref="A1:K21" xr:uid="{5C2EF26B-8F7C-40DC-90B6-805AC60B672A}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{65BC4CFE-CBD1-4A0C-ACAB-8E0C8A33A81F}" name="Table1" displayName="Table1" ref="A1:K24" totalsRowShown="0" headerRowDxfId="1">
+  <autoFilter ref="A1:K24" xr:uid="{5C2EF26B-8F7C-40DC-90B6-805AC60B672A}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K18">
     <sortCondition ref="A1:A18"/>
   </sortState>
@@ -2001,8 +2037,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CEB7023-1E9A-48AE-8417-31A8A140F136}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T13" sqref="T13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="S15" sqref="S15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2014,25 +2050,24 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F901F93A-6EBC-444E-BB8F-D0008D03E2AA}">
-  <dimension ref="A1:K21"/>
+  <dimension ref="A1:K24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J21" sqref="J21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J24" sqref="J24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="10.19921875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.73046875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18.1328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.1328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.19921875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.19921875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.53125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.796875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.796875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="6.9296875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.265625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.73046875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.86328125" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.45">
@@ -2611,7 +2646,7 @@
         <v>186</v>
       </c>
       <c r="J16">
-        <f>SUM(B16:I16)</f>
+        <f t="shared" ref="J16:J21" si="1">SUM(B16:I16)</f>
         <v>9110</v>
       </c>
       <c r="K16">
@@ -2647,7 +2682,7 @@
         <v>186</v>
       </c>
       <c r="J17">
-        <f>SUM(B17:I17)</f>
+        <f t="shared" si="1"/>
         <v>9286</v>
       </c>
       <c r="K17">
@@ -2683,11 +2718,11 @@
         <v>186</v>
       </c>
       <c r="J18">
-        <f>SUM(B18:I18)</f>
+        <f t="shared" si="1"/>
         <v>10624</v>
       </c>
       <c r="K18">
-        <f>J18-J17</f>
+        <f t="shared" ref="K18:K23" si="2">J18-J17</f>
         <v>1338</v>
       </c>
     </row>
@@ -2720,11 +2755,11 @@
         <v>186</v>
       </c>
       <c r="J19">
-        <f>SUM(B19:I19)</f>
+        <f t="shared" si="1"/>
         <v>10959</v>
       </c>
       <c r="K19">
-        <f>J19-J18</f>
+        <f t="shared" si="2"/>
         <v>335</v>
       </c>
     </row>
@@ -2757,11 +2792,11 @@
         <v>186</v>
       </c>
       <c r="J20">
-        <f>SUM(B20:I20)</f>
+        <f t="shared" si="1"/>
         <v>11958</v>
       </c>
       <c r="K20">
-        <f>J20-J19</f>
+        <f t="shared" si="2"/>
         <v>999</v>
       </c>
     </row>
@@ -2794,12 +2829,123 @@
         <v>186</v>
       </c>
       <c r="J21">
-        <f>SUM(B21:I21)</f>
+        <f t="shared" si="1"/>
         <v>12014</v>
       </c>
       <c r="K21">
-        <f>J21-J20</f>
+        <f t="shared" si="2"/>
         <v>56</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A22" s="1">
+        <v>44155</v>
+      </c>
+      <c r="B22">
+        <v>236</v>
+      </c>
+      <c r="C22">
+        <v>87</v>
+      </c>
+      <c r="D22">
+        <v>516</v>
+      </c>
+      <c r="E22">
+        <v>7413</v>
+      </c>
+      <c r="F22">
+        <v>4475</v>
+      </c>
+      <c r="G22">
+        <v>120</v>
+      </c>
+      <c r="H22">
+        <v>117</v>
+      </c>
+      <c r="I22">
+        <v>186</v>
+      </c>
+      <c r="J22">
+        <f>SUM(B22:I22)</f>
+        <v>13150</v>
+      </c>
+      <c r="K22">
+        <f t="shared" si="2"/>
+        <v>1136</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A23" s="1">
+        <v>44156</v>
+      </c>
+      <c r="B23">
+        <v>236</v>
+      </c>
+      <c r="C23">
+        <v>87</v>
+      </c>
+      <c r="D23">
+        <v>516</v>
+      </c>
+      <c r="E23">
+        <v>7413</v>
+      </c>
+      <c r="F23">
+        <v>5154</v>
+      </c>
+      <c r="G23">
+        <v>120</v>
+      </c>
+      <c r="H23">
+        <v>117</v>
+      </c>
+      <c r="I23">
+        <v>186</v>
+      </c>
+      <c r="J23">
+        <f>SUM(B23:I23)</f>
+        <v>13829</v>
+      </c>
+      <c r="K23">
+        <f t="shared" si="2"/>
+        <v>679</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A24" s="1">
+        <v>44157</v>
+      </c>
+      <c r="B24">
+        <v>236</v>
+      </c>
+      <c r="C24">
+        <v>87</v>
+      </c>
+      <c r="D24">
+        <v>516</v>
+      </c>
+      <c r="E24">
+        <v>7413</v>
+      </c>
+      <c r="F24">
+        <v>5621</v>
+      </c>
+      <c r="G24">
+        <v>120</v>
+      </c>
+      <c r="H24">
+        <v>117</v>
+      </c>
+      <c r="I24">
+        <v>186</v>
+      </c>
+      <c r="J24">
+        <f>SUM(B24:I24)</f>
+        <v>14296</v>
+      </c>
+      <c r="K24">
+        <f>J24-J23</f>
+        <v>467</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Section 2.3.2.2: Reference-predication asymmetries
</commit_message>
<xml_diff>
--- a/thesis/progress.xlsx
+++ b/thesis/progress.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f7cf2c9d3dc7fdc6/Dissertation/thesis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="335" documentId="8_{8233B9E9-5E46-417E-8631-6A32EFB57DCE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{01BCFF38-A078-4402-A560-BBF6CEE25074}"/>
+  <xr:revisionPtr revIDLastSave="346" documentId="8_{8233B9E9-5E46-417E-8631-6A32EFB57DCE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{4D2B4C77-FA2E-425A-A441-EA74D41AB4E9}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{90EBE93A-7825-427E-BCBE-4711C8076B47}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="dashboard" sheetId="3" r:id="rId1"/>
     <sheet name="writing" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191028" calcCompleted="0"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -333,10 +333,10 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>writing!$A$2:$A$25</c:f>
+              <c:f>writing!$A$2:$A$26</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="24"/>
+                <c:ptCount val="25"/>
                 <c:pt idx="0">
                   <c:v>44130</c:v>
                 </c:pt>
@@ -408,16 +408,19 @@
                 </c:pt>
                 <c:pt idx="23">
                   <c:v>44158</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>44159</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>writing!$K$2:$K$25</c:f>
+              <c:f>writing!$K$2:$K$26</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="24"/>
+                <c:ptCount val="25"/>
                 <c:pt idx="0">
                   <c:v>1360</c:v>
                 </c:pt>
@@ -489,6 +492,9 @@
                 </c:pt>
                 <c:pt idx="23">
                   <c:v>156</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>921</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -600,10 +606,10 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>writing!$A$2:$A$25</c:f>
+              <c:f>writing!$A$2:$A$26</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="24"/>
+                <c:ptCount val="25"/>
                 <c:pt idx="0">
                   <c:v>44130</c:v>
                 </c:pt>
@@ -675,16 +681,19 @@
                 </c:pt>
                 <c:pt idx="23">
                   <c:v>44158</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>44159</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>writing!$J$2:$J$25</c:f>
+              <c:f>writing!$J$2:$J$26</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="24"/>
+                <c:ptCount val="25"/>
                 <c:pt idx="0">
                   <c:v>2225</c:v>
                 </c:pt>
@@ -756,6 +765,9 @@
                 </c:pt>
                 <c:pt idx="23">
                   <c:v>15807</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>16728</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1724,8 +1736,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{65BC4CFE-CBD1-4A0C-ACAB-8E0C8A33A81F}" name="Table1" displayName="Table1" ref="A1:K25" totalsRowShown="0" headerRowDxfId="1">
-  <autoFilter ref="A1:K25" xr:uid="{5C2EF26B-8F7C-40DC-90B6-805AC60B672A}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{65BC4CFE-CBD1-4A0C-ACAB-8E0C8A33A81F}" name="Table1" displayName="Table1" ref="A1:K26" totalsRowShown="0" headerRowDxfId="1">
+  <autoFilter ref="A1:K26" xr:uid="{5C2EF26B-8F7C-40DC-90B6-805AC60B672A}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K18">
     <sortCondition ref="A1:A18"/>
   </sortState>
@@ -2062,10 +2074,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F901F93A-6EBC-444E-BB8F-D0008D03E2AA}">
-  <dimension ref="A1:K25"/>
+  <dimension ref="A1:K26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M8" sqref="M8"/>
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2997,6 +3009,43 @@
         <v>156</v>
       </c>
     </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A26" s="1">
+        <v>44159</v>
+      </c>
+      <c r="B26">
+        <v>236</v>
+      </c>
+      <c r="C26">
+        <v>87</v>
+      </c>
+      <c r="D26">
+        <v>516</v>
+      </c>
+      <c r="E26">
+        <v>7486</v>
+      </c>
+      <c r="F26">
+        <v>7980</v>
+      </c>
+      <c r="G26">
+        <v>120</v>
+      </c>
+      <c r="H26">
+        <v>117</v>
+      </c>
+      <c r="I26">
+        <v>186</v>
+      </c>
+      <c r="J26">
+        <f>SUM(B26:I26)</f>
+        <v>16728</v>
+      </c>
+      <c r="K26">
+        <f>J26-J25</f>
+        <v>921</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>

<commit_message>
Section 2.3.2.3: Locus of categoriality
</commit_message>
<xml_diff>
--- a/thesis/progress.xlsx
+++ b/thesis/progress.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f7cf2c9d3dc7fdc6/Dissertation/thesis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="346" documentId="8_{8233B9E9-5E46-417E-8631-6A32EFB57DCE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{4D2B4C77-FA2E-425A-A441-EA74D41AB4E9}"/>
+  <xr:revisionPtr revIDLastSave="348" documentId="8_{8233B9E9-5E46-417E-8631-6A32EFB57DCE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{2DA6EC75-BFCE-4B59-B9E6-84310721E0DD}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{90EBE93A-7825-427E-BCBE-4711C8076B47}"/>
   </bookViews>
@@ -494,7 +494,7 @@
                   <c:v>156</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>921</c:v>
+                  <c:v>1628</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -767,7 +767,7 @@
                   <c:v>15807</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>16728</c:v>
+                  <c:v>17435</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3023,10 +3023,10 @@
         <v>516</v>
       </c>
       <c r="E26">
-        <v>7486</v>
+        <v>7562</v>
       </c>
       <c r="F26">
-        <v>7980</v>
+        <v>8611</v>
       </c>
       <c r="G26">
         <v>120</v>
@@ -3039,11 +3039,11 @@
       </c>
       <c r="J26">
         <f>SUM(B26:I26)</f>
-        <v>16728</v>
+        <v>17435</v>
       </c>
       <c r="K26">
         <f>J26-J25</f>
-        <v>921</v>
+        <v>1628</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Section 2.3.3: Problems & critiques: Intro
</commit_message>
<xml_diff>
--- a/thesis/progress.xlsx
+++ b/thesis/progress.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f7cf2c9d3dc7fdc6/Dissertation/thesis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="355" documentId="8_{8233B9E9-5E46-417E-8631-6A32EFB57DCE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{6C38684D-0504-41CF-A652-570BFBB053E4}"/>
+  <xr:revisionPtr revIDLastSave="359" documentId="8_{8233B9E9-5E46-417E-8631-6A32EFB57DCE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{7992D86C-494C-48D6-91A2-8C93EB7361EC}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" activeTab="1" xr2:uid="{90EBE93A-7825-427E-BCBE-4711C8076B47}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{90EBE93A-7825-427E-BCBE-4711C8076B47}"/>
   </bookViews>
   <sheets>
     <sheet name="dashboard" sheetId="3" r:id="rId1"/>
@@ -333,10 +333,10 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>writing!$A$2:$A$27</c:f>
+              <c:f>writing!$A$2:$A$28</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="26"/>
+                <c:ptCount val="27"/>
                 <c:pt idx="0">
                   <c:v>44130</c:v>
                 </c:pt>
@@ -414,16 +414,19 @@
                 </c:pt>
                 <c:pt idx="25">
                   <c:v>44160</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>44161</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>writing!$K$2:$K$27</c:f>
+              <c:f>writing!$K$2:$K$28</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="26"/>
+                <c:ptCount val="27"/>
                 <c:pt idx="0">
                   <c:v>1360</c:v>
                 </c:pt>
@@ -501,6 +504,9 @@
                 </c:pt>
                 <c:pt idx="25">
                   <c:v>905</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>203</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -612,10 +618,10 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>writing!$A$2:$A$27</c:f>
+              <c:f>writing!$A$2:$A$28</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="26"/>
+                <c:ptCount val="27"/>
                 <c:pt idx="0">
                   <c:v>44130</c:v>
                 </c:pt>
@@ -693,16 +699,19 @@
                 </c:pt>
                 <c:pt idx="25">
                   <c:v>44160</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>44161</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>writing!$J$2:$J$27</c:f>
+              <c:f>writing!$J$2:$J$28</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="26"/>
+                <c:ptCount val="27"/>
                 <c:pt idx="0">
                   <c:v>2225</c:v>
                 </c:pt>
@@ -780,6 +789,9 @@
                 </c:pt>
                 <c:pt idx="25">
                   <c:v>18340</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>18543</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1748,8 +1760,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{65BC4CFE-CBD1-4A0C-ACAB-8E0C8A33A81F}" name="Table1" displayName="Table1" ref="A1:K27" totalsRowShown="0" headerRowDxfId="1">
-  <autoFilter ref="A1:K27" xr:uid="{5C2EF26B-8F7C-40DC-90B6-805AC60B672A}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{65BC4CFE-CBD1-4A0C-ACAB-8E0C8A33A81F}" name="Table1" displayName="Table1" ref="A1:K28" totalsRowShown="0" headerRowDxfId="1">
+  <autoFilter ref="A1:K28" xr:uid="{5C2EF26B-8F7C-40DC-90B6-805AC60B672A}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K18">
     <sortCondition ref="A1:A18"/>
   </sortState>
@@ -2073,7 +2085,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CEB7023-1E9A-48AE-8417-31A8A140F136}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="R12" sqref="R12"/>
     </sheetView>
   </sheetViews>
@@ -2086,10 +2098,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F901F93A-6EBC-444E-BB8F-D0008D03E2AA}">
-  <dimension ref="A1:K27"/>
+  <dimension ref="A1:K28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3095,6 +3107,43 @@
         <v>905</v>
       </c>
     </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A28" s="1">
+        <v>44161</v>
+      </c>
+      <c r="B28">
+        <v>236</v>
+      </c>
+      <c r="C28">
+        <v>87</v>
+      </c>
+      <c r="D28">
+        <v>516</v>
+      </c>
+      <c r="E28">
+        <v>7562</v>
+      </c>
+      <c r="F28">
+        <v>9719</v>
+      </c>
+      <c r="G28">
+        <v>120</v>
+      </c>
+      <c r="H28">
+        <v>117</v>
+      </c>
+      <c r="I28">
+        <v>186</v>
+      </c>
+      <c r="J28">
+        <f>SUM(B28:I28)</f>
+        <v>18543</v>
+      </c>
+      <c r="K28">
+        <f>J28-J27</f>
+        <v>203</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>

<commit_message>
Sec. 2.3.3.1: Methodological opportunism
</commit_message>
<xml_diff>
--- a/thesis/progress.xlsx
+++ b/thesis/progress.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f7cf2c9d3dc7fdc6/Dissertation/thesis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="359" documentId="8_{8233B9E9-5E46-417E-8631-6A32EFB57DCE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{7992D86C-494C-48D6-91A2-8C93EB7361EC}"/>
+  <xr:revisionPtr revIDLastSave="363" documentId="8_{8233B9E9-5E46-417E-8631-6A32EFB57DCE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{EE3303C7-2B05-42FB-9405-41C5EF731496}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{90EBE93A-7825-427E-BCBE-4711C8076B47}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" activeTab="1" xr2:uid="{90EBE93A-7825-427E-BCBE-4711C8076B47}"/>
   </bookViews>
   <sheets>
     <sheet name="dashboard" sheetId="3" r:id="rId1"/>
     <sheet name="writing" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="191028" calcCompleted="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -333,10 +333,10 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>writing!$A$2:$A$28</c:f>
+              <c:f>writing!$A$2:$A$29</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="27"/>
+                <c:ptCount val="28"/>
                 <c:pt idx="0">
                   <c:v>44130</c:v>
                 </c:pt>
@@ -417,16 +417,19 @@
                 </c:pt>
                 <c:pt idx="26">
                   <c:v>44161</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>44162</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>writing!$K$2:$K$28</c:f>
+              <c:f>writing!$K$2:$K$29</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="27"/>
+                <c:ptCount val="28"/>
                 <c:pt idx="0">
                   <c:v>1360</c:v>
                 </c:pt>
@@ -507,6 +510,9 @@
                 </c:pt>
                 <c:pt idx="26">
                   <c:v>203</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>362</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -618,10 +624,10 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>writing!$A$2:$A$28</c:f>
+              <c:f>writing!$A$2:$A$29</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="27"/>
+                <c:ptCount val="28"/>
                 <c:pt idx="0">
                   <c:v>44130</c:v>
                 </c:pt>
@@ -702,16 +708,19 @@
                 </c:pt>
                 <c:pt idx="26">
                   <c:v>44161</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>44162</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>writing!$J$2:$J$28</c:f>
+              <c:f>writing!$J$2:$J$29</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="27"/>
+                <c:ptCount val="28"/>
                 <c:pt idx="0">
                   <c:v>2225</c:v>
                 </c:pt>
@@ -792,6 +801,9 @@
                 </c:pt>
                 <c:pt idx="26">
                   <c:v>18543</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>18905</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1760,8 +1772,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{65BC4CFE-CBD1-4A0C-ACAB-8E0C8A33A81F}" name="Table1" displayName="Table1" ref="A1:K28" totalsRowShown="0" headerRowDxfId="1">
-  <autoFilter ref="A1:K28" xr:uid="{5C2EF26B-8F7C-40DC-90B6-805AC60B672A}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{65BC4CFE-CBD1-4A0C-ACAB-8E0C8A33A81F}" name="Table1" displayName="Table1" ref="A1:K29" totalsRowShown="0" headerRowDxfId="1">
+  <autoFilter ref="A1:K29" xr:uid="{5C2EF26B-8F7C-40DC-90B6-805AC60B672A}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K18">
     <sortCondition ref="A1:A18"/>
   </sortState>
@@ -2085,7 +2097,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CEB7023-1E9A-48AE-8417-31A8A140F136}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="R12" sqref="R12"/>
     </sheetView>
   </sheetViews>
@@ -2098,10 +2110,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F901F93A-6EBC-444E-BB8F-D0008D03E2AA}">
-  <dimension ref="A1:K28"/>
+  <dimension ref="A1:K29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H28" sqref="H28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3144,6 +3156,43 @@
         <v>203</v>
       </c>
     </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A29" s="1">
+        <v>44162</v>
+      </c>
+      <c r="B29">
+        <v>236</v>
+      </c>
+      <c r="C29">
+        <v>87</v>
+      </c>
+      <c r="D29">
+        <v>516</v>
+      </c>
+      <c r="E29">
+        <v>7562</v>
+      </c>
+      <c r="F29">
+        <v>10081</v>
+      </c>
+      <c r="G29">
+        <v>120</v>
+      </c>
+      <c r="H29">
+        <v>117</v>
+      </c>
+      <c r="I29">
+        <v>186</v>
+      </c>
+      <c r="J29">
+        <f>SUM(B29:I29)</f>
+        <v>18905</v>
+      </c>
+      <c r="K29">
+        <f>J29-J28</f>
+        <v>362</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>

<commit_message>
Section 2.3.3: Problems & critiques
</commit_message>
<xml_diff>
--- a/thesis/progress.xlsx
+++ b/thesis/progress.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f7cf2c9d3dc7fdc6/Dissertation/thesis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="363" documentId="8_{8233B9E9-5E46-417E-8631-6A32EFB57DCE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{EE3303C7-2B05-42FB-9405-41C5EF731496}"/>
+  <xr:revisionPtr revIDLastSave="367" documentId="8_{8233B9E9-5E46-417E-8631-6A32EFB57DCE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{B8B2F021-CA55-42A9-8DA6-268D4B23D2BC}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" activeTab="1" xr2:uid="{90EBE93A-7825-427E-BCBE-4711C8076B47}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{90EBE93A-7825-427E-BCBE-4711C8076B47}"/>
   </bookViews>
   <sheets>
     <sheet name="dashboard" sheetId="3" r:id="rId1"/>
     <sheet name="writing" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191028" calcCompleted="0"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -333,10 +333,10 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>writing!$A$2:$A$29</c:f>
+              <c:f>writing!$A$2:$A$30</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="28"/>
+                <c:ptCount val="29"/>
                 <c:pt idx="0">
                   <c:v>44130</c:v>
                 </c:pt>
@@ -420,16 +420,19 @@
                 </c:pt>
                 <c:pt idx="27">
                   <c:v>44162</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>44163</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>writing!$K$2:$K$29</c:f>
+              <c:f>writing!$K$2:$K$30</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="28"/>
+                <c:ptCount val="29"/>
                 <c:pt idx="0">
                   <c:v>1360</c:v>
                 </c:pt>
@@ -513,6 +516,9 @@
                 </c:pt>
                 <c:pt idx="27">
                   <c:v>362</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>2964</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -624,10 +630,10 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>writing!$A$2:$A$29</c:f>
+              <c:f>writing!$A$2:$A$30</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="28"/>
+                <c:ptCount val="29"/>
                 <c:pt idx="0">
                   <c:v>44130</c:v>
                 </c:pt>
@@ -711,16 +717,19 @@
                 </c:pt>
                 <c:pt idx="27">
                   <c:v>44162</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>44163</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>writing!$J$2:$J$29</c:f>
+              <c:f>writing!$J$2:$J$30</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="28"/>
+                <c:ptCount val="29"/>
                 <c:pt idx="0">
                   <c:v>2225</c:v>
                 </c:pt>
@@ -804,6 +813,9 @@
                 </c:pt>
                 <c:pt idx="27">
                   <c:v>18905</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>21869</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1772,8 +1784,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{65BC4CFE-CBD1-4A0C-ACAB-8E0C8A33A81F}" name="Table1" displayName="Table1" ref="A1:K29" totalsRowShown="0" headerRowDxfId="1">
-  <autoFilter ref="A1:K29" xr:uid="{5C2EF26B-8F7C-40DC-90B6-805AC60B672A}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{65BC4CFE-CBD1-4A0C-ACAB-8E0C8A33A81F}" name="Table1" displayName="Table1" ref="A1:K30" totalsRowShown="0" headerRowDxfId="1">
+  <autoFilter ref="A1:K30" xr:uid="{5C2EF26B-8F7C-40DC-90B6-805AC60B672A}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K18">
     <sortCondition ref="A1:A18"/>
   </sortState>
@@ -2097,7 +2109,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CEB7023-1E9A-48AE-8417-31A8A140F136}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="R12" sqref="R12"/>
     </sheetView>
   </sheetViews>
@@ -2110,10 +2122,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F901F93A-6EBC-444E-BB8F-D0008D03E2AA}">
-  <dimension ref="A1:K29"/>
+  <dimension ref="A1:K30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3004,7 +3016,7 @@
         <v>15651</v>
       </c>
       <c r="K24">
-        <f>J24-J23</f>
+        <f t="shared" ref="K24:K29" si="4">J24-J23</f>
         <v>1822</v>
       </c>
     </row>
@@ -3041,7 +3053,7 @@
         <v>15807</v>
       </c>
       <c r="K25">
-        <f>J25-J24</f>
+        <f t="shared" si="4"/>
         <v>156</v>
       </c>
     </row>
@@ -3078,7 +3090,7 @@
         <v>17435</v>
       </c>
       <c r="K26">
-        <f>J26-J25</f>
+        <f t="shared" si="4"/>
         <v>1628</v>
       </c>
     </row>
@@ -3115,7 +3127,7 @@
         <v>18340</v>
       </c>
       <c r="K27">
-        <f>J27-J26</f>
+        <f t="shared" si="4"/>
         <v>905</v>
       </c>
     </row>
@@ -3152,7 +3164,7 @@
         <v>18543</v>
       </c>
       <c r="K28">
-        <f>J28-J27</f>
+        <f t="shared" si="4"/>
         <v>203</v>
       </c>
     </row>
@@ -3189,8 +3201,45 @@
         <v>18905</v>
       </c>
       <c r="K29">
-        <f>J29-J28</f>
+        <f t="shared" si="4"/>
         <v>362</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A30" s="1">
+        <v>44163</v>
+      </c>
+      <c r="B30">
+        <v>236</v>
+      </c>
+      <c r="C30">
+        <v>87</v>
+      </c>
+      <c r="D30">
+        <v>516</v>
+      </c>
+      <c r="E30">
+        <v>7574</v>
+      </c>
+      <c r="F30">
+        <v>13033</v>
+      </c>
+      <c r="G30">
+        <v>120</v>
+      </c>
+      <c r="H30">
+        <v>117</v>
+      </c>
+      <c r="I30">
+        <v>186</v>
+      </c>
+      <c r="J30">
+        <f>SUM(B30:I30)</f>
+        <v>21869</v>
+      </c>
+      <c r="K30">
+        <f>J30-J29</f>
+        <v>2964</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Lexical flexibility: A functional definition
</commit_message>
<xml_diff>
--- a/thesis/progress.xlsx
+++ b/thesis/progress.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f7cf2c9d3dc7fdc6/Dissertation/thesis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="387" documentId="8_{8233B9E9-5E46-417E-8631-6A32EFB57DCE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{82BCE20D-1DA2-40EE-91E3-7DA2AD134B72}"/>
+  <xr:revisionPtr revIDLastSave="388" documentId="8_{8233B9E9-5E46-417E-8631-6A32EFB57DCE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{AF7CA987-8C76-4CDE-A821-20BDFB582B20}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{90EBE93A-7825-427E-BCBE-4711C8076B47}"/>
   </bookViews>
@@ -536,7 +536,7 @@
                   <c:v>1336</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>688</c:v>
+                  <c:v>2389</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -851,7 +851,7 @@
                   <c:v>25077</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>25765</c:v>
+                  <c:v>27466</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2161,7 +2161,7 @@
   <dimension ref="A1:K33"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="G33" sqref="G33:I33"/>
+      <selection activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3196,7 +3196,7 @@
         <v>186</v>
       </c>
       <c r="J28">
-        <f>SUM(B28:I28)</f>
+        <f t="shared" ref="J28:J33" si="5">SUM(B28:I28)</f>
         <v>18543</v>
       </c>
       <c r="K28">
@@ -3233,7 +3233,7 @@
         <v>186</v>
       </c>
       <c r="J29">
-        <f>SUM(B29:I29)</f>
+        <f t="shared" si="5"/>
         <v>18905</v>
       </c>
       <c r="K29">
@@ -3270,7 +3270,7 @@
         <v>186</v>
       </c>
       <c r="J30">
-        <f>SUM(B30:I30)</f>
+        <f t="shared" si="5"/>
         <v>21869</v>
       </c>
       <c r="K30">
@@ -3307,7 +3307,7 @@
         <v>186</v>
       </c>
       <c r="J31">
-        <f>SUM(B31:I31)</f>
+        <f t="shared" si="5"/>
         <v>23741</v>
       </c>
       <c r="K31">
@@ -3344,7 +3344,7 @@
         <v>186</v>
       </c>
       <c r="J32">
-        <f>SUM(B32:I32)</f>
+        <f t="shared" si="5"/>
         <v>25077</v>
       </c>
       <c r="K32">
@@ -3369,7 +3369,7 @@
         <v>7723</v>
       </c>
       <c r="F33">
-        <v>16780</v>
+        <v>18481</v>
       </c>
       <c r="G33">
         <v>120</v>
@@ -3381,12 +3381,12 @@
         <v>186</v>
       </c>
       <c r="J33">
-        <f>SUM(B33:I33)</f>
-        <v>25765</v>
+        <f t="shared" si="5"/>
+        <v>27466</v>
       </c>
       <c r="K33">
         <f>J33-J32</f>
-        <v>688</v>
+        <v>2389</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Ch. 2 MM edits
</commit_message>
<xml_diff>
--- a/thesis/progress.xlsx
+++ b/thesis/progress.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f7cf2c9d3dc7fdc6/Dissertation/thesis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="473" documentId="8_{8233B9E9-5E46-417E-8631-6A32EFB57DCE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{3F2BFBE3-C233-402A-A310-C7FB6D30982A}"/>
+  <xr:revisionPtr revIDLastSave="484" documentId="8_{8233B9E9-5E46-417E-8631-6A32EFB57DCE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{38D92726-694C-4A26-A6F6-61DEE65B8363}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" activeTab="1" xr2:uid="{90EBE93A-7825-427E-BCBE-4711C8076B47}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{90EBE93A-7825-427E-BCBE-4711C8076B47}"/>
   </bookViews>
   <sheets>
     <sheet name="dashboard" sheetId="3" r:id="rId1"/>
@@ -345,10 +345,10 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>writing!$A$2:$A$39</c:f>
+              <c:f>writing!$A$2:$A$41</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="38"/>
+                <c:ptCount val="40"/>
                 <c:pt idx="0">
                   <c:v>44130</c:v>
                 </c:pt>
@@ -462,16 +462,22 @@
                 </c:pt>
                 <c:pt idx="37">
                   <c:v>44175</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>44176</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>44177</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>writing!$N$2:$N$39</c:f>
+              <c:f>writing!$N$2:$N$41</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="38"/>
+                <c:ptCount val="40"/>
                 <c:pt idx="0">
                   <c:v>1360</c:v>
                 </c:pt>
@@ -585,6 +591,12 @@
                 </c:pt>
                 <c:pt idx="37">
                   <c:v>129</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>137</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>511</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -696,10 +708,10 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>writing!$A$2:$A$39</c:f>
+              <c:f>writing!$A$2:$A$41</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="38"/>
+                <c:ptCount val="40"/>
                 <c:pt idx="0">
                   <c:v>44130</c:v>
                 </c:pt>
@@ -813,16 +825,22 @@
                 </c:pt>
                 <c:pt idx="37">
                   <c:v>44175</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>44176</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>44177</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>writing!$M$2:$M$39</c:f>
+              <c:f>writing!$M$2:$M$41</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="38"/>
+                <c:ptCount val="40"/>
                 <c:pt idx="0">
                   <c:v>2614</c:v>
                 </c:pt>
@@ -936,6 +954,12 @@
                 </c:pt>
                 <c:pt idx="37">
                   <c:v>29577</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>29714</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>30225</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1870,7 +1894,7 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>26</xdr:col>
+      <xdr:col>27</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>30</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -1904,8 +1928,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{65BC4CFE-CBD1-4A0C-ACAB-8E0C8A33A81F}" name="Table1" displayName="Table1" ref="A1:N39" totalsRowShown="0" headerRowDxfId="2">
-  <autoFilter ref="A1:N39" xr:uid="{5C2EF26B-8F7C-40DC-90B6-805AC60B672A}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{65BC4CFE-CBD1-4A0C-ACAB-8E0C8A33A81F}" name="Table1" displayName="Table1" ref="A1:N41" totalsRowShown="0" headerRowDxfId="2">
+  <autoFilter ref="A1:N41" xr:uid="{5C2EF26B-8F7C-40DC-90B6-805AC60B672A}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:N18">
     <sortCondition ref="A1:A18"/>
   </sortState>
@@ -2232,8 +2256,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CEB7023-1E9A-48AE-8417-31A8A140F136}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="S16" sqref="S16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Z33" sqref="Z33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2245,10 +2269,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F901F93A-6EBC-444E-BB8F-D0008D03E2AA}">
-  <dimension ref="A1:N39"/>
+  <dimension ref="A1:N41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="I39" sqref="I39"/>
+    <sheetView topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="J41" sqref="J41:L41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3862,7 +3886,7 @@
         <v>186</v>
       </c>
       <c r="M35">
-        <f>SUM(C35:L35)</f>
+        <f t="shared" ref="M35:M40" si="2">SUM(C35:L35)</f>
         <v>29649</v>
       </c>
       <c r="N35" cm="1">
@@ -3908,7 +3932,7 @@
         <v>186</v>
       </c>
       <c r="M36">
-        <f>SUM(C36:L36)</f>
+        <f t="shared" si="2"/>
         <v>29649</v>
       </c>
       <c r="N36" cm="1">
@@ -3954,7 +3978,7 @@
         <v>186</v>
       </c>
       <c r="M37">
-        <f>SUM(C37:L37)</f>
+        <f t="shared" si="2"/>
         <v>29196</v>
       </c>
       <c r="N37" cm="1">
@@ -4000,7 +4024,7 @@
         <v>186</v>
       </c>
       <c r="M38">
-        <f>SUM(C38:L38)</f>
+        <f t="shared" si="2"/>
         <v>29448</v>
       </c>
       <c r="N38" cm="1">
@@ -4046,12 +4070,104 @@
         <v>186</v>
       </c>
       <c r="M39">
-        <f>SUM(C39:L39)</f>
+        <f t="shared" si="2"/>
         <v>29577</v>
       </c>
       <c r="N39" cm="1">
         <f t="array" ref="N39">SUM(ABS(C39:L39-C38:L38))</f>
         <v>129</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A40" s="1">
+        <v>44176</v>
+      </c>
+      <c r="B40">
+        <v>568</v>
+      </c>
+      <c r="C40">
+        <v>239</v>
+      </c>
+      <c r="D40">
+        <v>87</v>
+      </c>
+      <c r="E40">
+        <v>198</v>
+      </c>
+      <c r="F40">
+        <v>492</v>
+      </c>
+      <c r="G40">
+        <v>416</v>
+      </c>
+      <c r="H40">
+        <v>8074</v>
+      </c>
+      <c r="I40">
+        <v>19786</v>
+      </c>
+      <c r="J40">
+        <v>120</v>
+      </c>
+      <c r="K40">
+        <v>116</v>
+      </c>
+      <c r="L40">
+        <v>186</v>
+      </c>
+      <c r="M40">
+        <f t="shared" si="2"/>
+        <v>29714</v>
+      </c>
+      <c r="N40">
+        <f>M40-M39</f>
+        <v>137</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A41" s="1">
+        <v>44177</v>
+      </c>
+      <c r="B41">
+        <v>568</v>
+      </c>
+      <c r="C41">
+        <v>239</v>
+      </c>
+      <c r="D41">
+        <v>87</v>
+      </c>
+      <c r="E41">
+        <v>198</v>
+      </c>
+      <c r="F41">
+        <v>492</v>
+      </c>
+      <c r="G41">
+        <v>416</v>
+      </c>
+      <c r="H41">
+        <v>8506</v>
+      </c>
+      <c r="I41">
+        <v>19865</v>
+      </c>
+      <c r="J41">
+        <v>120</v>
+      </c>
+      <c r="K41">
+        <v>116</v>
+      </c>
+      <c r="L41">
+        <v>186</v>
+      </c>
+      <c r="M41">
+        <f>SUM(C41:L41)</f>
+        <v>30225</v>
+      </c>
+      <c r="N41">
+        <f>M41-M40</f>
+        <v>511</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
revisions: Ch. 1 & Ch. 2
</commit_message>
<xml_diff>
--- a/thesis/progress.xlsx
+++ b/thesis/progress.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f7cf2c9d3dc7fdc6/Dissertation/thesis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="462" documentId="8_{8233B9E9-5E46-417E-8631-6A32EFB57DCE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{374E9537-1254-46EA-B8F6-FCF72BFE24DB}"/>
+  <xr:revisionPtr revIDLastSave="490" documentId="8_{8233B9E9-5E46-417E-8631-6A32EFB57DCE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{BF15400B-8A26-4490-A955-AE812D1798BA}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{90EBE93A-7825-427E-BCBE-4711C8076B47}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{90EBE93A-7825-427E-BCBE-4711C8076B47}"/>
   </bookViews>
   <sheets>
     <sheet name="dashboard" sheetId="3" r:id="rId1"/>
     <sheet name="writing" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191028" calcCompleted="0"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -345,10 +345,10 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>writing!$A$2:$A$37</c:f>
+              <c:f>writing!$A$2:$A$42</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="36"/>
+                <c:ptCount val="41"/>
                 <c:pt idx="0">
                   <c:v>44130</c:v>
                 </c:pt>
@@ -456,16 +456,31 @@
                 </c:pt>
                 <c:pt idx="35">
                   <c:v>44173</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>44174</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>44175</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>44176</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>44177</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>44178</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>writing!$N$2:$N$37</c:f>
+              <c:f>writing!$N$2:$N$42</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="36"/>
+                <c:ptCount val="41"/>
                 <c:pt idx="0">
                   <c:v>1360</c:v>
                 </c:pt>
@@ -573,6 +588,21 @@
                 </c:pt>
                 <c:pt idx="35">
                   <c:v>463</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>252</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>129</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>137</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>511</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -684,10 +714,10 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>writing!$A$2:$A$37</c:f>
+              <c:f>writing!$A$2:$A$42</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="36"/>
+                <c:ptCount val="41"/>
                 <c:pt idx="0">
                   <c:v>44130</c:v>
                 </c:pt>
@@ -795,16 +825,31 @@
                 </c:pt>
                 <c:pt idx="35">
                   <c:v>44173</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>44174</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>44175</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>44176</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>44177</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>44178</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>writing!$M$2:$M$37</c:f>
+              <c:f>writing!$M$2:$M$42</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="36"/>
+                <c:ptCount val="41"/>
                 <c:pt idx="0">
                   <c:v>2614</c:v>
                 </c:pt>
@@ -912,6 +957,21 @@
                 </c:pt>
                 <c:pt idx="35">
                   <c:v>29196</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>29448</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>29577</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>29714</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>30225</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>30224</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1846,10 +1906,10 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>195262</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1880,8 +1940,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{65BC4CFE-CBD1-4A0C-ACAB-8E0C8A33A81F}" name="Table1" displayName="Table1" ref="A1:N37" totalsRowShown="0" headerRowDxfId="2">
-  <autoFilter ref="A1:N37" xr:uid="{5C2EF26B-8F7C-40DC-90B6-805AC60B672A}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{65BC4CFE-CBD1-4A0C-ACAB-8E0C8A33A81F}" name="Table1" displayName="Table1" ref="A1:N42" totalsRowShown="0" headerRowDxfId="2">
+  <autoFilter ref="A1:N42" xr:uid="{5C2EF26B-8F7C-40DC-90B6-805AC60B672A}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:N18">
     <sortCondition ref="A1:A18"/>
   </sortState>
@@ -2209,7 +2269,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S16" sqref="S16"/>
+      <selection activeCell="P33" sqref="P33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2221,10 +2281,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F901F93A-6EBC-444E-BB8F-D0008D03E2AA}">
-  <dimension ref="A1:N37"/>
+  <dimension ref="A1:N42"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="L37" sqref="L37"/>
+    <sheetView topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="M41" sqref="M41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3838,7 +3898,7 @@
         <v>186</v>
       </c>
       <c r="M35">
-        <f>SUM(C35:L35)</f>
+        <f t="shared" ref="M35:M40" si="2">SUM(C35:L35)</f>
         <v>29649</v>
       </c>
       <c r="N35" cm="1">
@@ -3884,7 +3944,7 @@
         <v>186</v>
       </c>
       <c r="M36">
-        <f>SUM(C36:L36)</f>
+        <f t="shared" si="2"/>
         <v>29649</v>
       </c>
       <c r="N36" cm="1">
@@ -3930,12 +3990,242 @@
         <v>186</v>
       </c>
       <c r="M37">
-        <f>SUM(C37:L37)</f>
+        <f t="shared" si="2"/>
         <v>29196</v>
       </c>
       <c r="N37" cm="1">
         <f t="array" ref="N37">SUM(ABS(C37:L37-C36:L36))</f>
         <v>463</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A38" s="1">
+        <v>44174</v>
+      </c>
+      <c r="B38">
+        <v>568</v>
+      </c>
+      <c r="C38">
+        <v>239</v>
+      </c>
+      <c r="D38">
+        <v>87</v>
+      </c>
+      <c r="E38">
+        <v>198</v>
+      </c>
+      <c r="F38">
+        <v>492</v>
+      </c>
+      <c r="G38">
+        <v>416</v>
+      </c>
+      <c r="H38">
+        <v>7945</v>
+      </c>
+      <c r="I38">
+        <v>19649</v>
+      </c>
+      <c r="J38">
+        <v>120</v>
+      </c>
+      <c r="K38">
+        <v>116</v>
+      </c>
+      <c r="L38">
+        <v>186</v>
+      </c>
+      <c r="M38">
+        <f t="shared" si="2"/>
+        <v>29448</v>
+      </c>
+      <c r="N38" cm="1">
+        <f t="array" ref="N38">SUM(ABS(C38:L38-C37:L37))</f>
+        <v>252</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A39" s="1">
+        <v>44175</v>
+      </c>
+      <c r="B39">
+        <v>568</v>
+      </c>
+      <c r="C39">
+        <v>239</v>
+      </c>
+      <c r="D39">
+        <v>87</v>
+      </c>
+      <c r="E39">
+        <v>198</v>
+      </c>
+      <c r="F39">
+        <v>492</v>
+      </c>
+      <c r="G39">
+        <v>416</v>
+      </c>
+      <c r="H39">
+        <v>8074</v>
+      </c>
+      <c r="I39">
+        <v>19649</v>
+      </c>
+      <c r="J39">
+        <v>120</v>
+      </c>
+      <c r="K39">
+        <v>116</v>
+      </c>
+      <c r="L39">
+        <v>186</v>
+      </c>
+      <c r="M39">
+        <f t="shared" si="2"/>
+        <v>29577</v>
+      </c>
+      <c r="N39" cm="1">
+        <f t="array" ref="N39">SUM(ABS(C39:L39-C38:L38))</f>
+        <v>129</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A40" s="1">
+        <v>44176</v>
+      </c>
+      <c r="B40">
+        <v>568</v>
+      </c>
+      <c r="C40">
+        <v>239</v>
+      </c>
+      <c r="D40">
+        <v>87</v>
+      </c>
+      <c r="E40">
+        <v>198</v>
+      </c>
+      <c r="F40">
+        <v>492</v>
+      </c>
+      <c r="G40">
+        <v>416</v>
+      </c>
+      <c r="H40">
+        <v>8074</v>
+      </c>
+      <c r="I40">
+        <v>19786</v>
+      </c>
+      <c r="J40">
+        <v>120</v>
+      </c>
+      <c r="K40">
+        <v>116</v>
+      </c>
+      <c r="L40">
+        <v>186</v>
+      </c>
+      <c r="M40">
+        <f t="shared" si="2"/>
+        <v>29714</v>
+      </c>
+      <c r="N40" cm="1">
+        <f t="array" ref="N40">SUM(ABS(C40:L40-C39:L39))</f>
+        <v>137</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A41" s="1">
+        <v>44177</v>
+      </c>
+      <c r="B41">
+        <v>568</v>
+      </c>
+      <c r="C41">
+        <v>239</v>
+      </c>
+      <c r="D41">
+        <v>87</v>
+      </c>
+      <c r="E41">
+        <v>198</v>
+      </c>
+      <c r="F41">
+        <v>492</v>
+      </c>
+      <c r="G41">
+        <v>416</v>
+      </c>
+      <c r="H41">
+        <v>8506</v>
+      </c>
+      <c r="I41">
+        <v>19865</v>
+      </c>
+      <c r="J41">
+        <v>120</v>
+      </c>
+      <c r="K41">
+        <v>116</v>
+      </c>
+      <c r="L41">
+        <v>186</v>
+      </c>
+      <c r="M41">
+        <f>SUM(C41:L41)</f>
+        <v>30225</v>
+      </c>
+      <c r="N41" cm="1">
+        <f t="array" ref="N41">SUM(ABS(C41:L41-C40:L40))</f>
+        <v>511</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A42" s="1">
+        <v>44178</v>
+      </c>
+      <c r="B42">
+        <v>568</v>
+      </c>
+      <c r="C42">
+        <v>239</v>
+      </c>
+      <c r="D42">
+        <v>87</v>
+      </c>
+      <c r="E42">
+        <v>198</v>
+      </c>
+      <c r="F42">
+        <v>492</v>
+      </c>
+      <c r="G42">
+        <v>416</v>
+      </c>
+      <c r="H42">
+        <v>8506</v>
+      </c>
+      <c r="I42">
+        <v>19864</v>
+      </c>
+      <c r="J42">
+        <v>120</v>
+      </c>
+      <c r="K42">
+        <v>116</v>
+      </c>
+      <c r="L42">
+        <v>186</v>
+      </c>
+      <c r="M42">
+        <f>SUM(C42:L42)</f>
+        <v>30224</v>
+      </c>
+      <c r="N42" cm="1">
+        <f t="array" ref="N42">SUM(ABS(C42:L42-C41:L41))</f>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Section 3.4.1: Measuring lexical flexibility
</commit_message>
<xml_diff>
--- a/thesis/progress.xlsx
+++ b/thesis/progress.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f7cf2c9d3dc7fdc6/Dissertation/thesis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="512" documentId="8_{8233B9E9-5E46-417E-8631-6A32EFB57DCE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{020EF252-1379-4FA7-880B-58B17FF757A3}"/>
+  <xr:revisionPtr revIDLastSave="517" documentId="8_{8233B9E9-5E46-417E-8631-6A32EFB57DCE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{C3950674-FDFE-4ECB-9BBD-DC5D47CCE28E}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{90EBE93A-7825-427E-BCBE-4711C8076B47}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" activeTab="1" xr2:uid="{90EBE93A-7825-427E-BCBE-4711C8076B47}"/>
   </bookViews>
   <sheets>
     <sheet name="dashboard" sheetId="3" r:id="rId1"/>
@@ -345,10 +345,10 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>writing!$A$2:$A$46</c:f>
+              <c:f>writing!$A$2:$A$47</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="45"/>
+                <c:ptCount val="46"/>
                 <c:pt idx="0">
                   <c:v>44130</c:v>
                 </c:pt>
@@ -483,16 +483,19 @@
                 </c:pt>
                 <c:pt idx="44">
                   <c:v>44182</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>44189</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>writing!$N$2:$N$46</c:f>
+              <c:f>writing!$N$2:$N$47</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="45"/>
+                <c:ptCount val="46"/>
                 <c:pt idx="0">
                   <c:v>1360</c:v>
                 </c:pt>
@@ -627,6 +630,9 @@
                 </c:pt>
                 <c:pt idx="44">
                   <c:v>1159</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>828</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -738,10 +744,10 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>writing!$A$2:$A$46</c:f>
+              <c:f>writing!$A$2:$A$47</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="45"/>
+                <c:ptCount val="46"/>
                 <c:pt idx="0">
                   <c:v>44130</c:v>
                 </c:pt>
@@ -876,16 +882,19 @@
                 </c:pt>
                 <c:pt idx="44">
                   <c:v>44182</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>44189</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>writing!$M$2:$M$46</c:f>
+              <c:f>writing!$M$2:$M$47</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="45"/>
+                <c:ptCount val="46"/>
                 <c:pt idx="0">
                   <c:v>2614</c:v>
                 </c:pt>
@@ -1020,6 +1029,9 @@
                 </c:pt>
                 <c:pt idx="44">
                   <c:v>33773</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>34601</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1988,8 +2000,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{65BC4CFE-CBD1-4A0C-ACAB-8E0C8A33A81F}" name="Table1" displayName="Table1" ref="A1:N46" totalsRowShown="0" headerRowDxfId="2">
-  <autoFilter ref="A1:N46" xr:uid="{5C2EF26B-8F7C-40DC-90B6-805AC60B672A}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{65BC4CFE-CBD1-4A0C-ACAB-8E0C8A33A81F}" name="Table1" displayName="Table1" ref="A1:N47" totalsRowShown="0" headerRowDxfId="2">
+  <autoFilter ref="A1:N47" xr:uid="{5C2EF26B-8F7C-40DC-90B6-805AC60B672A}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:N18">
     <sortCondition ref="A1:A18"/>
   </sortState>
@@ -2316,7 +2328,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CEB7023-1E9A-48AE-8417-31A8A140F136}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="P33" sqref="P33"/>
     </sheetView>
   </sheetViews>
@@ -2329,10 +2341,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F901F93A-6EBC-444E-BB8F-D0008D03E2AA}">
-  <dimension ref="A1:N46"/>
+  <dimension ref="A1:N47"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="K46" sqref="K46:L46"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="K44" sqref="K44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -4222,7 +4234,7 @@
         <v>186</v>
       </c>
       <c r="M41">
-        <f>SUM(C41:L41)</f>
+        <f t="shared" ref="M41:M46" si="3">SUM(C41:L41)</f>
         <v>30225</v>
       </c>
       <c r="N41" cm="1">
@@ -4268,7 +4280,7 @@
         <v>186</v>
       </c>
       <c r="M42">
-        <f>SUM(C42:L42)</f>
+        <f t="shared" si="3"/>
         <v>30224</v>
       </c>
       <c r="N42" cm="1">
@@ -4314,11 +4326,11 @@
         <v>186</v>
       </c>
       <c r="M43">
-        <f>SUM(C43:L43)</f>
+        <f t="shared" si="3"/>
         <v>30597</v>
       </c>
-      <c r="N43">
-        <f>M43-M42</f>
+      <c r="N43" cm="1">
+        <f t="array" ref="N43">SUM(ABS(C43:L43-C42:L42))</f>
         <v>373</v>
       </c>
     </row>
@@ -4360,11 +4372,11 @@
         <v>186</v>
       </c>
       <c r="M44">
-        <f>SUM(C44:L44)</f>
+        <f t="shared" si="3"/>
         <v>31305</v>
       </c>
-      <c r="N44">
-        <f>M44-M43</f>
+      <c r="N44" cm="1">
+        <f t="array" ref="N44">SUM(ABS(C44:L44-C43:L43))</f>
         <v>708</v>
       </c>
     </row>
@@ -4406,11 +4418,11 @@
         <v>186</v>
       </c>
       <c r="M45">
-        <f>SUM(C45:L45)</f>
+        <f t="shared" si="3"/>
         <v>32614</v>
       </c>
-      <c r="N45">
-        <f>M45-M44</f>
+      <c r="N45" cm="1">
+        <f t="array" ref="N45">SUM(ABS(C45:L45-C44:L44))</f>
         <v>1309</v>
       </c>
     </row>
@@ -4452,12 +4464,58 @@
         <v>186</v>
       </c>
       <c r="M46">
-        <f>SUM(C46:L46)</f>
+        <f t="shared" si="3"/>
         <v>33773</v>
       </c>
-      <c r="N46">
-        <f>M46-M45</f>
+      <c r="N46" cm="1">
+        <f t="array" ref="N46">SUM(ABS(C46:L46-C45:L45))</f>
         <v>1159</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A47" s="1">
+        <v>44189</v>
+      </c>
+      <c r="B47">
+        <v>568</v>
+      </c>
+      <c r="C47">
+        <v>239</v>
+      </c>
+      <c r="D47">
+        <v>87</v>
+      </c>
+      <c r="E47">
+        <v>198</v>
+      </c>
+      <c r="F47">
+        <v>492</v>
+      </c>
+      <c r="G47">
+        <v>416</v>
+      </c>
+      <c r="H47">
+        <v>8524</v>
+      </c>
+      <c r="I47">
+        <v>19896</v>
+      </c>
+      <c r="J47">
+        <v>4447</v>
+      </c>
+      <c r="K47">
+        <v>116</v>
+      </c>
+      <c r="L47">
+        <v>186</v>
+      </c>
+      <c r="M47">
+        <f>SUM(C47:L47)</f>
+        <v>34601</v>
+      </c>
+      <c r="N47" cm="1">
+        <f t="array" ref="N47">SUM(ABS(C47:L47-C46:L46))</f>
+        <v>828</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Appendix C: sample annotations
</commit_message>
<xml_diff>
--- a/thesis/progress.xlsx
+++ b/thesis/progress.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f7cf2c9d3dc7fdc6/Dissertation/thesis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="567" documentId="8_{8233B9E9-5E46-417E-8631-6A32EFB57DCE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{4956A7C5-72D1-4F1B-827E-2C537E62D803}"/>
+  <xr:revisionPtr revIDLastSave="575" documentId="8_{8233B9E9-5E46-417E-8631-6A32EFB57DCE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{152839AF-9948-4374-BAE2-CE5D5653F561}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{90EBE93A-7825-427E-BCBE-4711C8076B47}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="dashboard" sheetId="3" r:id="rId1"/>
     <sheet name="writing" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="191028" calcCompleted="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -354,10 +354,10 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>writing!$A$2:$A$49</c:f>
+              <c:f>writing!$A$2:$A$50</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="48"/>
+                <c:ptCount val="49"/>
                 <c:pt idx="0">
                   <c:v>44130</c:v>
                 </c:pt>
@@ -501,16 +501,19 @@
                 </c:pt>
                 <c:pt idx="47">
                   <c:v>44195</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>44197</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>writing!$Q$2:$Q$49</c:f>
+              <c:f>writing!$Q$2:$Q$50</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="48"/>
+                <c:ptCount val="49"/>
                 <c:pt idx="0">
                   <c:v>1360</c:v>
                 </c:pt>
@@ -654,6 +657,9 @@
                 </c:pt>
                 <c:pt idx="47">
                   <c:v>3837</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>1323</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -765,10 +771,10 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>writing!$A$2:$A$49</c:f>
+              <c:f>writing!$A$2:$A$50</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="48"/>
+                <c:ptCount val="49"/>
                 <c:pt idx="0">
                   <c:v>44130</c:v>
                 </c:pt>
@@ -912,16 +918,19 @@
                 </c:pt>
                 <c:pt idx="47">
                   <c:v>44195</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>44197</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>writing!$P$2:$P$49</c:f>
+              <c:f>writing!$P$2:$P$50</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="48"/>
+                <c:ptCount val="49"/>
                 <c:pt idx="0">
                   <c:v>2614</c:v>
                 </c:pt>
@@ -1065,6 +1074,9 @@
                 </c:pt>
                 <c:pt idx="47">
                   <c:v>40046</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>41369</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2033,8 +2045,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{65BC4CFE-CBD1-4A0C-ACAB-8E0C8A33A81F}" name="Table1" displayName="Table1" ref="A1:Q49" totalsRowShown="0" headerRowDxfId="2">
-  <autoFilter ref="A1:Q49" xr:uid="{5C2EF26B-8F7C-40DC-90B6-805AC60B672A}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{65BC4CFE-CBD1-4A0C-ACAB-8E0C8A33A81F}" name="Table1" displayName="Table1" ref="A1:Q50" totalsRowShown="0" headerRowDxfId="2">
+  <autoFilter ref="A1:Q50" xr:uid="{5C2EF26B-8F7C-40DC-90B6-805AC60B672A}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:Q18">
     <sortCondition ref="A1:A18"/>
   </sortState>
@@ -2365,7 +2377,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P33" sqref="P33"/>
+      <selection activeCell="S35" sqref="S35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2377,10 +2389,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F901F93A-6EBC-444E-BB8F-D0008D03E2AA}">
-  <dimension ref="A1:Q49"/>
+  <dimension ref="A1:Q50"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="P2" sqref="P2:P49"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="L50" sqref="L50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -5094,6 +5106,61 @@
         <v>3837</v>
       </c>
     </row>
+    <row r="50" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="A50" s="1">
+        <v>44197</v>
+      </c>
+      <c r="B50">
+        <v>568</v>
+      </c>
+      <c r="C50">
+        <v>239</v>
+      </c>
+      <c r="D50">
+        <v>87</v>
+      </c>
+      <c r="E50">
+        <v>229</v>
+      </c>
+      <c r="F50">
+        <v>492</v>
+      </c>
+      <c r="G50">
+        <v>416</v>
+      </c>
+      <c r="H50">
+        <v>8498</v>
+      </c>
+      <c r="I50">
+        <v>19876</v>
+      </c>
+      <c r="J50">
+        <v>5844</v>
+      </c>
+      <c r="K50">
+        <v>117</v>
+      </c>
+      <c r="L50">
+        <v>186</v>
+      </c>
+      <c r="M50">
+        <v>497</v>
+      </c>
+      <c r="N50">
+        <v>3559</v>
+      </c>
+      <c r="O50">
+        <v>1329</v>
+      </c>
+      <c r="P50">
+        <f>SUM(C50:O50)</f>
+        <v>41369</v>
+      </c>
+      <c r="Q50" cm="1">
+        <f t="array" ref="Q50">SUM(ABS(C50:O50-C49:O49))</f>
+        <v>1323</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>

<commit_message>
Ch. 3: Methods [draft]
</commit_message>
<xml_diff>
--- a/thesis/progress.xlsx
+++ b/thesis/progress.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f7cf2c9d3dc7fdc6/Dissertation/thesis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="490" documentId="8_{8233B9E9-5E46-417E-8631-6A32EFB57DCE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{BF15400B-8A26-4490-A955-AE812D1798BA}"/>
+  <xr:revisionPtr revIDLastSave="592" documentId="8_{8233B9E9-5E46-417E-8631-6A32EFB57DCE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{ABCA1320-68BE-3B4E-9554-DC5B7F8111C8}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{90EBE93A-7825-427E-BCBE-4711C8076B47}"/>
   </bookViews>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Date</t>
   </si>
@@ -99,6 +99,15 @@
   </si>
   <si>
     <t>CV</t>
+  </si>
+  <si>
+    <t>App: Grammars</t>
+  </si>
+  <si>
+    <t>App: 100-items</t>
+  </si>
+  <si>
+    <t>App: Annotations</t>
   </si>
 </sst>
 </file>
@@ -152,10 +161,10 @@
   </cellStyles>
   <dxfs count="3">
     <dxf>
-      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+      <numFmt numFmtId="164" formatCode="m/d/yyyy"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+      <numFmt numFmtId="164" formatCode="m/d/yyyy"/>
     </dxf>
     <dxf>
       <font>
@@ -269,7 +278,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>writing!$N$1</c:f>
+              <c:f>writing!$Q$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -345,10 +354,10 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>writing!$A$2:$A$42</c:f>
+              <c:f>writing!$A$2:$A$51</c:f>
               <c:numCache>
-                <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="41"/>
+                <c:formatCode>m/d/yy</c:formatCode>
+                <c:ptCount val="50"/>
                 <c:pt idx="0">
                   <c:v>44130</c:v>
                 </c:pt>
@@ -471,16 +480,43 @@
                 </c:pt>
                 <c:pt idx="40">
                   <c:v>44178</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>44179</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>44180</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>44181</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>44182</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>44189</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>44194</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>44195</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>44197</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>44198</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>writing!$N$2:$N$42</c:f>
+              <c:f>writing!$Q$2:$Q$51</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="41"/>
+                <c:ptCount val="50"/>
                 <c:pt idx="0">
                   <c:v>1360</c:v>
                 </c:pt>
@@ -500,7 +536,7 @@
                   <c:v>1511</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>621</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>811</c:v>
@@ -515,19 +551,19 @@
                   <c:v>439</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>584</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>843</c:v>
+                  <c:v>511</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>511</c:v>
+                  <c:v>1582</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>2671</c:v>
+                  <c:v>1582</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>577</c:v>
+                  <c:v>176</c:v>
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>1406</c:v>
@@ -563,7 +599,7 @@
                   <c:v>203</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>362</c:v>
+                  <c:v>859</c:v>
                 </c:pt>
                 <c:pt idx="28">
                   <c:v>2964</c:v>
@@ -603,6 +639,33 @@
                 </c:pt>
                 <c:pt idx="40">
                   <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>373</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>708</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>1309</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>1175</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>828</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>1187</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>3837</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>1323</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>350</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -633,7 +696,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>writing!$M$1</c:f>
+              <c:f>writing!$P$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -714,10 +777,10 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>writing!$A$2:$A$42</c:f>
+              <c:f>writing!$A$2:$A$51</c:f>
               <c:numCache>
-                <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="41"/>
+                <c:formatCode>m/d/yy</c:formatCode>
+                <c:ptCount val="50"/>
                 <c:pt idx="0">
                   <c:v>44130</c:v>
                 </c:pt>
@@ -840,16 +903,43 @@
                 </c:pt>
                 <c:pt idx="40">
                   <c:v>44178</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>44179</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>44180</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>44181</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>44182</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>44189</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>44194</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>44195</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>44197</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>44198</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>writing!$M$2:$M$42</c:f>
+              <c:f>writing!$P$2:$P$51</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="41"/>
+                <c:ptCount val="50"/>
                 <c:pt idx="0">
                   <c:v>2614</c:v>
                 </c:pt>
@@ -890,7 +980,7 @@
                   <c:v>9499</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>9110</c:v>
+                  <c:v>11013</c:v>
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>9499</c:v>
@@ -932,46 +1022,73 @@
                   <c:v>18932</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>19294</c:v>
+                  <c:v>19791</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>22258</c:v>
+                  <c:v>22755</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>24130</c:v>
+                  <c:v>24627</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>25466</c:v>
+                  <c:v>25963</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>27855</c:v>
+                  <c:v>28352</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>29646</c:v>
+                  <c:v>30143</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>29649</c:v>
+                  <c:v>30146</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>29649</c:v>
+                  <c:v>30146</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>29196</c:v>
+                  <c:v>29693</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>29448</c:v>
+                  <c:v>29945</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>29577</c:v>
+                  <c:v>30074</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>29714</c:v>
+                  <c:v>30211</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>30225</c:v>
+                  <c:v>30722</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>30224</c:v>
+                  <c:v>30721</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>31094</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>31802</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>33111</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>34286</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>35114</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>36301</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>40046</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>41369</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>41719</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1003,7 +1120,7 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
+        <c:numFmt formatCode="m/d/yy" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1261,7 +1378,7 @@
         </c:scaling>
         <c:delete val="1"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
+        <c:numFmt formatCode="m/d/yy" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1907,7 +2024,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>27</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:colOff>218966</xdr:colOff>
       <xdr:row>30</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
@@ -1940,12 +2057,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{65BC4CFE-CBD1-4A0C-ACAB-8E0C8A33A81F}" name="Table1" displayName="Table1" ref="A1:N42" totalsRowShown="0" headerRowDxfId="2">
-  <autoFilter ref="A1:N42" xr:uid="{5C2EF26B-8F7C-40DC-90B6-805AC60B672A}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:N18">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{65BC4CFE-CBD1-4A0C-ACAB-8E0C8A33A81F}" name="Table1" displayName="Table1" ref="A1:Q51" totalsRowShown="0" headerRowDxfId="2">
+  <autoFilter ref="A1:Q51" xr:uid="{5C2EF26B-8F7C-40DC-90B6-805AC60B672A}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:Q18">
     <sortCondition ref="A1:A18"/>
   </sortState>
-  <tableColumns count="14">
+  <tableColumns count="17">
     <tableColumn id="1" xr3:uid="{BEA871B4-EEE2-4F93-9DBC-4AFC40E06E5F}" name="Date" dataDxfId="1"/>
     <tableColumn id="15" xr3:uid="{1B7B50EE-D1EF-4405-B2B9-09BEA9C0CE20}" name="CV" dataDxfId="0"/>
     <tableColumn id="2" xr3:uid="{3081B1F4-64BE-4187-A6E1-DC702177CD85}" name="Abstract"/>
@@ -1958,11 +2075,14 @@
     <tableColumn id="7" xr3:uid="{DBDA4A9C-3B12-453F-B457-620D99362FF4}" name="3: Data &amp; Methods"/>
     <tableColumn id="8" xr3:uid="{C2A4C48B-7471-4014-9277-4A1B1EF3B40B}" name="4: Results"/>
     <tableColumn id="9" xr3:uid="{58756D61-0637-4214-BD00-EE98CC70539C}" name="5: Conclusion"/>
+    <tableColumn id="14" xr3:uid="{A0B27E14-9B88-430C-9991-860F493F768F}" name="App: Grammars"/>
+    <tableColumn id="16" xr3:uid="{070AEEBA-EE16-4E1A-AEF6-19497CCE82B9}" name="App: 100-items"/>
+    <tableColumn id="17" xr3:uid="{BE87AA87-E374-40DC-9D81-405C193B82BF}" name="App: Annotations"/>
     <tableColumn id="10" xr3:uid="{457CFC5C-BE64-406D-A9FB-BB2DBEA65B42}" name="Total">
-      <calculatedColumnFormula>SUM(C2:L2)</calculatedColumnFormula>
+      <calculatedColumnFormula>SUM(C2:O2)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="11" xr3:uid="{778E3DE4-F274-4416-84BC-FF498402E770}" name="Daily">
-      <calculatedColumnFormula>M2-M1</calculatedColumnFormula>
+      <calculatedColumnFormula>P2-P1</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -2272,7 +2392,7 @@
       <selection activeCell="P33" sqref="P33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -2281,32 +2401,32 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F901F93A-6EBC-444E-BB8F-D0008D03E2AA}">
-  <dimension ref="A1:N42"/>
+  <dimension ref="A1:Q51"/>
   <sheetViews>
     <sheetView topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="M41" sqref="M41"/>
+      <selection activeCell="K46" sqref="K46:L46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.19921875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.06640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.73046875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.1328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.3984375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.1328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.22265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.68359375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.16015625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.390625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.43359375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.1796875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="15.19921875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.53125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.796875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.796875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="7" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="6.9296875" customWidth="1"/>
-    <col min="15" max="15" width="7" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.52734375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.29296875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.76171875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.94921875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16.54296875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="18.4296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2344,13 +2464,22 @@
         <v>8</v>
       </c>
       <c r="M1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="P1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="Q1" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>44130</v>
       </c>
@@ -2388,14 +2517,23 @@
         <v>0</v>
       </c>
       <c r="M2">
-        <f t="shared" ref="M2:M14" si="0">SUM(C2:L2)</f>
+        <v>0</v>
+      </c>
+      <c r="N2">
+        <v>0</v>
+      </c>
+      <c r="O2">
+        <v>0</v>
+      </c>
+      <c r="P2">
+        <f>SUM(C2:O2)</f>
         <v>2614</v>
       </c>
-      <c r="N2">
+      <c r="Q2">
         <v>1360</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>44131</v>
       </c>
@@ -2433,15 +2571,24 @@
         <v>0</v>
       </c>
       <c r="M3">
-        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N3">
+        <v>0</v>
+      </c>
+      <c r="O3">
+        <v>0</v>
+      </c>
+      <c r="P3">
+        <f>SUM(C3:O3)</f>
         <v>3628</v>
       </c>
-      <c r="N3" cm="1">
-        <f t="array" ref="N3">SUM(ABS(C3:L3-C2:L2))</f>
+      <c r="Q3" cm="1">
+        <f t="array" ref="Q3">SUM(ABS(C3:O3-C2:O2))</f>
         <v>1014</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>44132</v>
       </c>
@@ -2479,15 +2626,24 @@
         <v>0</v>
       </c>
       <c r="M4">
-        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N4">
+        <v>0</v>
+      </c>
+      <c r="O4">
+        <v>0</v>
+      </c>
+      <c r="P4">
+        <f>SUM(C4:O4)</f>
         <v>4429</v>
       </c>
-      <c r="N4" cm="1">
-        <f t="array" ref="N4">SUM(ABS(C4:L4-C3:L3))</f>
+      <c r="Q4" cm="1">
+        <f t="array" ref="Q4">SUM(ABS(C4:O4-C3:O3))</f>
         <v>801</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>44133</v>
       </c>
@@ -2525,15 +2681,24 @@
         <v>0</v>
       </c>
       <c r="M5">
-        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N5">
+        <v>0</v>
+      </c>
+      <c r="O5">
+        <v>0</v>
+      </c>
+      <c r="P5">
+        <f>SUM(C5:O5)</f>
         <v>5670</v>
       </c>
-      <c r="N5" cm="1">
-        <f t="array" ref="N5">SUM(ABS(C5:L5-C4:L4))</f>
+      <c r="Q5" cm="1">
+        <f t="array" ref="Q5">SUM(ABS(C5:O5-C4:O4))</f>
         <v>1241</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>44134</v>
       </c>
@@ -2571,15 +2736,24 @@
         <v>0</v>
       </c>
       <c r="M6">
-        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N6">
+        <v>0</v>
+      </c>
+      <c r="O6">
+        <v>0</v>
+      </c>
+      <c r="P6">
+        <f>SUM(C6:O6)</f>
         <v>6433</v>
       </c>
-      <c r="N6" cm="1">
-        <f t="array" ref="N6">SUM(ABS(C6:L6-C5:L5))</f>
+      <c r="Q6" cm="1">
+        <f t="array" ref="Q6">SUM(ABS(C6:O6-C5:O5))</f>
         <v>763</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>44135</v>
       </c>
@@ -2617,15 +2791,24 @@
         <v>5</v>
       </c>
       <c r="M7">
-        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N7">
+        <v>0</v>
+      </c>
+      <c r="O7">
+        <v>0</v>
+      </c>
+      <c r="P7">
+        <f>SUM(C7:O7)</f>
         <v>7922</v>
       </c>
-      <c r="N7" cm="1">
-        <f t="array" ref="N7">SUM(ABS(C7:L7-C6:L6))</f>
+      <c r="Q7" cm="1">
+        <f t="array" ref="Q7">SUM(ABS(C7:O7-C6:O6))</f>
         <v>1511</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>44136</v>
       </c>
@@ -2663,14 +2846,24 @@
         <v>5</v>
       </c>
       <c r="M8">
-        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N8">
+        <v>0</v>
+      </c>
+      <c r="O8">
+        <v>0</v>
+      </c>
+      <c r="P8">
+        <f>SUM(C8:O8)</f>
         <v>7922</v>
       </c>
-      <c r="N8">
-        <v>621</v>
+      <c r="Q8" cm="1">
+        <f t="array" ref="Q8">SUM(ABS(C8:O8-C7:O7))</f>
+        <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>44137</v>
       </c>
@@ -2708,15 +2901,24 @@
         <v>5</v>
       </c>
       <c r="M9">
-        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N9">
+        <v>0</v>
+      </c>
+      <c r="O9">
+        <v>0</v>
+      </c>
+      <c r="P9">
+        <f>SUM(C9:O9)</f>
         <v>8733</v>
       </c>
-      <c r="N9" cm="1">
-        <f t="array" ref="N9">SUM(ABS(C9:L9-C8:L8))</f>
+      <c r="Q9" cm="1">
+        <f t="array" ref="Q9">SUM(ABS(C9:O9-C8:O8))</f>
         <v>811</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>44138</v>
       </c>
@@ -2754,15 +2956,24 @@
         <v>5</v>
       </c>
       <c r="M10">
-        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N10">
+        <v>0</v>
+      </c>
+      <c r="O10">
+        <v>0</v>
+      </c>
+      <c r="P10">
+        <f>SUM(C10:O10)</f>
         <v>8943</v>
       </c>
-      <c r="N10" cm="1">
-        <f t="array" ref="N10">SUM(ABS(C10:L10-C9:L9))</f>
+      <c r="Q10" cm="1">
+        <f t="array" ref="Q10">SUM(ABS(C10:O10-C9:O9))</f>
         <v>210</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>44139</v>
       </c>
@@ -2800,15 +3011,24 @@
         <v>5</v>
       </c>
       <c r="M11">
-        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N11">
+        <v>0</v>
+      </c>
+      <c r="O11">
+        <v>0</v>
+      </c>
+      <c r="P11">
+        <f>SUM(C11:O11)</f>
         <v>8913</v>
       </c>
-      <c r="N11" cm="1">
-        <f t="array" ref="N11">SUM(ABS(C11:L11-C10:L10))</f>
+      <c r="Q11" cm="1">
+        <f t="array" ref="Q11">SUM(ABS(C11:O11-C10:O10))</f>
         <v>56</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>44142</v>
       </c>
@@ -2846,15 +3066,24 @@
         <v>5</v>
       </c>
       <c r="M12">
-        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N12">
+        <v>0</v>
+      </c>
+      <c r="O12">
+        <v>0</v>
+      </c>
+      <c r="P12">
+        <f>SUM(C12:O12)</f>
         <v>8988</v>
       </c>
-      <c r="N12" cm="1">
-        <f t="array" ref="N12">SUM(ABS(C12:L12-C11:L11))</f>
+      <c r="Q12" cm="1">
+        <f t="array" ref="Q12">SUM(ABS(C12:O12-C11:O11))</f>
         <v>439</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>44143</v>
       </c>
@@ -2892,14 +3121,24 @@
         <v>5</v>
       </c>
       <c r="M13">
-        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N13">
+        <v>0</v>
+      </c>
+      <c r="O13">
+        <v>0</v>
+      </c>
+      <c r="P13">
+        <f>SUM(C13:O13)</f>
         <v>8988</v>
       </c>
-      <c r="N13">
-        <v>584</v>
+      <c r="Q13" cm="1">
+        <f t="array" ref="Q13">SUM(ABS(C13:O13-C12:O12))</f>
+        <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>44144</v>
       </c>
@@ -2937,14 +3176,24 @@
         <v>186</v>
       </c>
       <c r="M14">
-        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N14">
+        <v>0</v>
+      </c>
+      <c r="O14">
+        <v>0</v>
+      </c>
+      <c r="P14">
+        <f>SUM(C14:O14)</f>
         <v>9499</v>
       </c>
-      <c r="N14">
-        <v>843</v>
+      <c r="Q14" cm="1">
+        <f t="array" ref="Q14">SUM(ABS(C14:O14-C13:O13))</f>
+        <v>511</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>44145</v>
       </c>
@@ -2982,13 +3231,24 @@
         <v>186</v>
       </c>
       <c r="M15">
-        <v>9110</v>
+        <v>0</v>
       </c>
       <c r="N15">
-        <v>511</v>
+        <v>0</v>
+      </c>
+      <c r="O15">
+        <v>0</v>
+      </c>
+      <c r="P15">
+        <f>SUM(C15:O15)</f>
+        <v>11013</v>
+      </c>
+      <c r="Q15" cm="1">
+        <f t="array" ref="Q15">SUM(ABS(C15:O15-C14:O14))</f>
+        <v>1582</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>44146</v>
       </c>
@@ -3026,14 +3286,24 @@
         <v>186</v>
       </c>
       <c r="M16">
-        <f t="shared" ref="M16:M34" si="1">SUM(C16:L16)</f>
+        <v>0</v>
+      </c>
+      <c r="N16">
+        <v>0</v>
+      </c>
+      <c r="O16">
+        <v>0</v>
+      </c>
+      <c r="P16">
+        <f>SUM(C16:O16)</f>
         <v>9499</v>
       </c>
-      <c r="N16">
-        <v>2671</v>
+      <c r="Q16" cm="1">
+        <f t="array" ref="Q16">SUM(ABS(C16:O16-C15:O15))</f>
+        <v>1582</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>44150</v>
       </c>
@@ -3071,14 +3341,24 @@
         <v>186</v>
       </c>
       <c r="M17">
-        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N17">
+        <v>0</v>
+      </c>
+      <c r="O17">
+        <v>0</v>
+      </c>
+      <c r="P17">
+        <f>SUM(C17:O17)</f>
         <v>9675</v>
       </c>
-      <c r="N17">
-        <v>577</v>
+      <c r="Q17" cm="1">
+        <f t="array" ref="Q17">SUM(ABS(C17:O17-C16:O16))</f>
+        <v>176</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>44151</v>
       </c>
@@ -3116,15 +3396,24 @@
         <v>186</v>
       </c>
       <c r="M18">
-        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N18">
+        <v>0</v>
+      </c>
+      <c r="O18">
+        <v>0</v>
+      </c>
+      <c r="P18">
+        <f>SUM(C18:O18)</f>
         <v>11013</v>
       </c>
-      <c r="N18" cm="1">
-        <f t="array" ref="N18">SUM(ABS(C18:L18-C17:L17))</f>
+      <c r="Q18" cm="1">
+        <f t="array" ref="Q18">SUM(ABS(C18:O18-C17:O17))</f>
         <v>1406</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>44152</v>
       </c>
@@ -3162,15 +3451,24 @@
         <v>186</v>
       </c>
       <c r="M19">
-        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N19">
+        <v>0</v>
+      </c>
+      <c r="O19">
+        <v>0</v>
+      </c>
+      <c r="P19">
+        <f>SUM(C19:O19)</f>
         <v>11348</v>
       </c>
-      <c r="N19" cm="1">
-        <f t="array" ref="N19">SUM(ABS(C19:L19-C18:L18))</f>
+      <c r="Q19" cm="1">
+        <f t="array" ref="Q19">SUM(ABS(C19:O19-C18:O18))</f>
         <v>335</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>44153</v>
       </c>
@@ -3208,15 +3506,24 @@
         <v>186</v>
       </c>
       <c r="M20">
-        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N20">
+        <v>0</v>
+      </c>
+      <c r="O20">
+        <v>0</v>
+      </c>
+      <c r="P20">
+        <f>SUM(C20:O20)</f>
         <v>12347</v>
       </c>
-      <c r="N20" cm="1">
-        <f t="array" ref="N20">SUM(ABS(C20:L20-C19:L19))</f>
+      <c r="Q20" cm="1">
+        <f t="array" ref="Q20">SUM(ABS(C20:O20-C19:O19))</f>
         <v>999</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>44154</v>
       </c>
@@ -3254,15 +3561,24 @@
         <v>186</v>
       </c>
       <c r="M21">
-        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N21">
+        <v>0</v>
+      </c>
+      <c r="O21">
+        <v>0</v>
+      </c>
+      <c r="P21">
+        <f>SUM(C21:O21)</f>
         <v>12403</v>
       </c>
-      <c r="N21" cm="1">
-        <f t="array" ref="N21">SUM(ABS(C21:L21-C20:L20))</f>
+      <c r="Q21" cm="1">
+        <f t="array" ref="Q21">SUM(ABS(C21:O21-C20:O20))</f>
         <v>56</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>44155</v>
       </c>
@@ -3300,15 +3616,24 @@
         <v>186</v>
       </c>
       <c r="M22">
-        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N22">
+        <v>0</v>
+      </c>
+      <c r="O22">
+        <v>0</v>
+      </c>
+      <c r="P22">
+        <f>SUM(C22:O22)</f>
         <v>13539</v>
       </c>
-      <c r="N22" cm="1">
-        <f t="array" ref="N22">SUM(ABS(C22:L22-C21:L21))</f>
+      <c r="Q22" cm="1">
+        <f t="array" ref="Q22">SUM(ABS(C22:O22-C21:O21))</f>
         <v>1136</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>44156</v>
       </c>
@@ -3346,15 +3671,24 @@
         <v>186</v>
       </c>
       <c r="M23">
-        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N23">
+        <v>0</v>
+      </c>
+      <c r="O23">
+        <v>0</v>
+      </c>
+      <c r="P23">
+        <f>SUM(C23:O23)</f>
         <v>14218</v>
       </c>
-      <c r="N23" cm="1">
-        <f t="array" ref="N23">SUM(ABS(C23:L23-C22:L22))</f>
+      <c r="Q23" cm="1">
+        <f t="array" ref="Q23">SUM(ABS(C23:O23-C22:O22))</f>
         <v>679</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>44157</v>
       </c>
@@ -3392,15 +3726,24 @@
         <v>186</v>
       </c>
       <c r="M24">
-        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N24">
+        <v>0</v>
+      </c>
+      <c r="O24">
+        <v>0</v>
+      </c>
+      <c r="P24">
+        <f>SUM(C24:O24)</f>
         <v>16040</v>
       </c>
-      <c r="N24" cm="1">
-        <f t="array" ref="N24">SUM(ABS(C24:L24-C23:L23))</f>
+      <c r="Q24" cm="1">
+        <f t="array" ref="Q24">SUM(ABS(C24:O24-C23:O23))</f>
         <v>1822</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <v>44158</v>
       </c>
@@ -3438,15 +3781,24 @@
         <v>186</v>
       </c>
       <c r="M25">
-        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N25">
+        <v>0</v>
+      </c>
+      <c r="O25">
+        <v>0</v>
+      </c>
+      <c r="P25">
+        <f>SUM(C25:O25)</f>
         <v>16196</v>
       </c>
-      <c r="N25" cm="1">
-        <f t="array" ref="N25">SUM(ABS(C25:L25-C24:L24))</f>
+      <c r="Q25" cm="1">
+        <f t="array" ref="Q25">SUM(ABS(C25:O25-C24:O24))</f>
         <v>156</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <v>44159</v>
       </c>
@@ -3484,15 +3836,24 @@
         <v>186</v>
       </c>
       <c r="M26">
-        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N26">
+        <v>0</v>
+      </c>
+      <c r="O26">
+        <v>0</v>
+      </c>
+      <c r="P26">
+        <f>SUM(C26:O26)</f>
         <v>17824</v>
       </c>
-      <c r="N26" cm="1">
-        <f t="array" ref="N26">SUM(ABS(C26:L26-C25:L25))</f>
+      <c r="Q26" cm="1">
+        <f t="array" ref="Q26">SUM(ABS(C26:O26-C25:O25))</f>
         <v>1628</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
         <v>44160</v>
       </c>
@@ -3530,15 +3891,24 @@
         <v>186</v>
       </c>
       <c r="M27">
-        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N27">
+        <v>0</v>
+      </c>
+      <c r="O27">
+        <v>0</v>
+      </c>
+      <c r="P27">
+        <f>SUM(C27:O27)</f>
         <v>18729</v>
       </c>
-      <c r="N27" cm="1">
-        <f t="array" ref="N27">SUM(ABS(C27:L27-C26:L26))</f>
+      <c r="Q27" cm="1">
+        <f t="array" ref="Q27">SUM(ABS(C27:O27-C26:O26))</f>
         <v>905</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
         <v>44161</v>
       </c>
@@ -3576,15 +3946,24 @@
         <v>186</v>
       </c>
       <c r="M28">
-        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N28">
+        <v>0</v>
+      </c>
+      <c r="O28">
+        <v>0</v>
+      </c>
+      <c r="P28">
+        <f>SUM(C28:O28)</f>
         <v>18932</v>
       </c>
-      <c r="N28" cm="1">
-        <f t="array" ref="N28">SUM(ABS(C28:L28-C27:L27))</f>
+      <c r="Q28" cm="1">
+        <f t="array" ref="Q28">SUM(ABS(C28:O28-C27:O27))</f>
         <v>203</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
         <v>44162</v>
       </c>
@@ -3622,15 +4001,24 @@
         <v>186</v>
       </c>
       <c r="M29">
-        <f t="shared" si="1"/>
-        <v>19294</v>
-      </c>
-      <c r="N29" cm="1">
-        <f t="array" ref="N29">SUM(ABS(C29:L29-C28:L28))</f>
-        <v>362</v>
+        <v>497</v>
+      </c>
+      <c r="N29">
+        <v>0</v>
+      </c>
+      <c r="O29">
+        <v>0</v>
+      </c>
+      <c r="P29">
+        <f>SUM(C29:O29)</f>
+        <v>19791</v>
+      </c>
+      <c r="Q29" cm="1">
+        <f t="array" ref="Q29">SUM(ABS(C29:O29-C28:O28))</f>
+        <v>859</v>
       </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
         <v>44163</v>
       </c>
@@ -3668,15 +4056,24 @@
         <v>186</v>
       </c>
       <c r="M30">
-        <f t="shared" si="1"/>
-        <v>22258</v>
-      </c>
-      <c r="N30" cm="1">
-        <f t="array" ref="N30">SUM(ABS(C30:L30-C29:L29))</f>
+        <v>497</v>
+      </c>
+      <c r="N30">
+        <v>0</v>
+      </c>
+      <c r="O30">
+        <v>0</v>
+      </c>
+      <c r="P30">
+        <f>SUM(C30:O30)</f>
+        <v>22755</v>
+      </c>
+      <c r="Q30" cm="1">
+        <f t="array" ref="Q30">SUM(ABS(C30:O30-C29:O29))</f>
         <v>2964</v>
       </c>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
         <v>44164</v>
       </c>
@@ -3714,15 +4111,24 @@
         <v>186</v>
       </c>
       <c r="M31">
-        <f t="shared" si="1"/>
-        <v>24130</v>
-      </c>
-      <c r="N31" cm="1">
-        <f t="array" ref="N31">SUM(ABS(C31:L31-C30:L30))</f>
+        <v>497</v>
+      </c>
+      <c r="N31">
+        <v>0</v>
+      </c>
+      <c r="O31">
+        <v>0</v>
+      </c>
+      <c r="P31">
+        <f>SUM(C31:O31)</f>
+        <v>24627</v>
+      </c>
+      <c r="Q31" cm="1">
+        <f t="array" ref="Q31">SUM(ABS(C31:O31-C30:O30))</f>
         <v>1872</v>
       </c>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
         <v>44166</v>
       </c>
@@ -3760,15 +4166,24 @@
         <v>186</v>
       </c>
       <c r="M32">
-        <f t="shared" si="1"/>
-        <v>25466</v>
-      </c>
-      <c r="N32" cm="1">
-        <f t="array" ref="N32">SUM(ABS(C32:L32-C31:L31))</f>
+        <v>497</v>
+      </c>
+      <c r="N32">
+        <v>0</v>
+      </c>
+      <c r="O32">
+        <v>0</v>
+      </c>
+      <c r="P32">
+        <f>SUM(C32:O32)</f>
+        <v>25963</v>
+      </c>
+      <c r="Q32" cm="1">
+        <f t="array" ref="Q32">SUM(ABS(C32:O32-C31:O31))</f>
         <v>1336</v>
       </c>
     </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
         <v>44167</v>
       </c>
@@ -3806,15 +4221,24 @@
         <v>186</v>
       </c>
       <c r="M33">
-        <f t="shared" si="1"/>
-        <v>27855</v>
-      </c>
-      <c r="N33" cm="1">
-        <f t="array" ref="N33">SUM(ABS(C33:L33-C32:L32))</f>
+        <v>497</v>
+      </c>
+      <c r="N33">
+        <v>0</v>
+      </c>
+      <c r="O33">
+        <v>0</v>
+      </c>
+      <c r="P33">
+        <f>SUM(C33:O33)</f>
+        <v>28352</v>
+      </c>
+      <c r="Q33" cm="1">
+        <f t="array" ref="Q33">SUM(ABS(C33:O33-C32:O32))</f>
         <v>2389</v>
       </c>
     </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
         <v>44168</v>
       </c>
@@ -3852,15 +4276,24 @@
         <v>186</v>
       </c>
       <c r="M34">
-        <f t="shared" si="1"/>
-        <v>29646</v>
-      </c>
-      <c r="N34" cm="1">
-        <f t="array" ref="N34">SUM(ABS(C34:L34-C33:L33))</f>
+        <v>497</v>
+      </c>
+      <c r="N34">
+        <v>0</v>
+      </c>
+      <c r="O34">
+        <v>0</v>
+      </c>
+      <c r="P34">
+        <f>SUM(C34:O34)</f>
+        <v>30143</v>
+      </c>
+      <c r="Q34" cm="1">
+        <f t="array" ref="Q34">SUM(ABS(C34:O34-C33:O33))</f>
         <v>1791</v>
       </c>
     </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
         <v>44169</v>
       </c>
@@ -3898,15 +4331,24 @@
         <v>186</v>
       </c>
       <c r="M35">
-        <f t="shared" ref="M35:M40" si="2">SUM(C35:L35)</f>
-        <v>29649</v>
-      </c>
-      <c r="N35" cm="1">
-        <f t="array" ref="N35">SUM(ABS(C35:L35-C34:L34))</f>
+        <v>497</v>
+      </c>
+      <c r="N35">
+        <v>0</v>
+      </c>
+      <c r="O35">
+        <v>0</v>
+      </c>
+      <c r="P35">
+        <f>SUM(C35:O35)</f>
+        <v>30146</v>
+      </c>
+      <c r="Q35" cm="1">
+        <f t="array" ref="Q35">SUM(ABS(C35:O35-C34:O34))</f>
         <v>481</v>
       </c>
     </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
         <v>44170</v>
       </c>
@@ -3944,15 +4386,24 @@
         <v>186</v>
       </c>
       <c r="M36">
-        <f t="shared" si="2"/>
-        <v>29649</v>
-      </c>
-      <c r="N36" cm="1">
-        <f t="array" ref="N36">SUM(ABS(C36:L36-C35:L35))</f>
+        <v>497</v>
+      </c>
+      <c r="N36">
+        <v>0</v>
+      </c>
+      <c r="O36">
+        <v>0</v>
+      </c>
+      <c r="P36">
+        <f>SUM(C36:O36)</f>
+        <v>30146</v>
+      </c>
+      <c r="Q36" cm="1">
+        <f t="array" ref="Q36">SUM(ABS(C36:O36-C35:O35))</f>
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
         <v>44173</v>
       </c>
@@ -3990,15 +4441,24 @@
         <v>186</v>
       </c>
       <c r="M37">
-        <f t="shared" si="2"/>
-        <v>29196</v>
-      </c>
-      <c r="N37" cm="1">
-        <f t="array" ref="N37">SUM(ABS(C37:L37-C36:L36))</f>
+        <v>497</v>
+      </c>
+      <c r="N37">
+        <v>0</v>
+      </c>
+      <c r="O37">
+        <v>0</v>
+      </c>
+      <c r="P37">
+        <f>SUM(C37:O37)</f>
+        <v>29693</v>
+      </c>
+      <c r="Q37" cm="1">
+        <f t="array" ref="Q37">SUM(ABS(C37:O37-C36:O36))</f>
         <v>463</v>
       </c>
     </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
         <v>44174</v>
       </c>
@@ -4036,15 +4496,24 @@
         <v>186</v>
       </c>
       <c r="M38">
-        <f t="shared" si="2"/>
-        <v>29448</v>
-      </c>
-      <c r="N38" cm="1">
-        <f t="array" ref="N38">SUM(ABS(C38:L38-C37:L37))</f>
+        <v>497</v>
+      </c>
+      <c r="N38">
+        <v>0</v>
+      </c>
+      <c r="O38">
+        <v>0</v>
+      </c>
+      <c r="P38">
+        <f>SUM(C38:O38)</f>
+        <v>29945</v>
+      </c>
+      <c r="Q38" cm="1">
+        <f t="array" ref="Q38">SUM(ABS(C38:O38-C37:O37))</f>
         <v>252</v>
       </c>
     </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A39" s="1">
         <v>44175</v>
       </c>
@@ -4082,15 +4551,24 @@
         <v>186</v>
       </c>
       <c r="M39">
-        <f t="shared" si="2"/>
-        <v>29577</v>
-      </c>
-      <c r="N39" cm="1">
-        <f t="array" ref="N39">SUM(ABS(C39:L39-C38:L38))</f>
+        <v>497</v>
+      </c>
+      <c r="N39">
+        <v>0</v>
+      </c>
+      <c r="O39">
+        <v>0</v>
+      </c>
+      <c r="P39">
+        <f>SUM(C39:O39)</f>
+        <v>30074</v>
+      </c>
+      <c r="Q39" cm="1">
+        <f t="array" ref="Q39">SUM(ABS(C39:O39-C38:O38))</f>
         <v>129</v>
       </c>
     </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A40" s="1">
         <v>44176</v>
       </c>
@@ -4128,15 +4606,24 @@
         <v>186</v>
       </c>
       <c r="M40">
-        <f t="shared" si="2"/>
-        <v>29714</v>
-      </c>
-      <c r="N40" cm="1">
-        <f t="array" ref="N40">SUM(ABS(C40:L40-C39:L39))</f>
+        <v>497</v>
+      </c>
+      <c r="N40">
+        <v>0</v>
+      </c>
+      <c r="O40">
+        <v>0</v>
+      </c>
+      <c r="P40">
+        <f>SUM(C40:O40)</f>
+        <v>30211</v>
+      </c>
+      <c r="Q40" cm="1">
+        <f t="array" ref="Q40">SUM(ABS(C40:O40-C39:O39))</f>
         <v>137</v>
       </c>
     </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A41" s="1">
         <v>44177</v>
       </c>
@@ -4174,15 +4661,24 @@
         <v>186</v>
       </c>
       <c r="M41">
-        <f>SUM(C41:L41)</f>
-        <v>30225</v>
-      </c>
-      <c r="N41" cm="1">
-        <f t="array" ref="N41">SUM(ABS(C41:L41-C40:L40))</f>
+        <v>497</v>
+      </c>
+      <c r="N41">
+        <v>0</v>
+      </c>
+      <c r="O41">
+        <v>0</v>
+      </c>
+      <c r="P41">
+        <f>SUM(C41:O41)</f>
+        <v>30722</v>
+      </c>
+      <c r="Q41" cm="1">
+        <f t="array" ref="Q41">SUM(ABS(C41:O41-C40:O40))</f>
         <v>511</v>
       </c>
     </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A42" s="1">
         <v>44178</v>
       </c>
@@ -4220,12 +4716,516 @@
         <v>186</v>
       </c>
       <c r="M42">
-        <f>SUM(C42:L42)</f>
-        <v>30224</v>
-      </c>
-      <c r="N42" cm="1">
-        <f t="array" ref="N42">SUM(ABS(C42:L42-C41:L41))</f>
+        <v>497</v>
+      </c>
+      <c r="N42">
+        <v>0</v>
+      </c>
+      <c r="O42">
+        <v>0</v>
+      </c>
+      <c r="P42">
+        <f>SUM(C42:O42)</f>
+        <v>30721</v>
+      </c>
+      <c r="Q42" cm="1">
+        <f t="array" ref="Q42">SUM(ABS(C42:O42-C41:O41))</f>
         <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A43" s="1">
+        <v>44179</v>
+      </c>
+      <c r="B43">
+        <v>568</v>
+      </c>
+      <c r="C43">
+        <v>239</v>
+      </c>
+      <c r="D43">
+        <v>87</v>
+      </c>
+      <c r="E43">
+        <v>198</v>
+      </c>
+      <c r="F43">
+        <v>492</v>
+      </c>
+      <c r="G43">
+        <v>416</v>
+      </c>
+      <c r="H43">
+        <v>8506</v>
+      </c>
+      <c r="I43">
+        <v>19864</v>
+      </c>
+      <c r="J43">
+        <v>493</v>
+      </c>
+      <c r="K43">
+        <v>116</v>
+      </c>
+      <c r="L43">
+        <v>186</v>
+      </c>
+      <c r="M43">
+        <v>497</v>
+      </c>
+      <c r="N43">
+        <v>0</v>
+      </c>
+      <c r="O43">
+        <v>0</v>
+      </c>
+      <c r="P43">
+        <f>SUM(C43:O43)</f>
+        <v>31094</v>
+      </c>
+      <c r="Q43" cm="1">
+        <f t="array" ref="Q43">SUM(ABS(C43:O43-C42:O42))</f>
+        <v>373</v>
+      </c>
+    </row>
+    <row r="44" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A44" s="1">
+        <v>44180</v>
+      </c>
+      <c r="B44">
+        <v>568</v>
+      </c>
+      <c r="C44">
+        <v>239</v>
+      </c>
+      <c r="D44">
+        <v>87</v>
+      </c>
+      <c r="E44">
+        <v>198</v>
+      </c>
+      <c r="F44">
+        <v>492</v>
+      </c>
+      <c r="G44">
+        <v>416</v>
+      </c>
+      <c r="H44">
+        <v>8506</v>
+      </c>
+      <c r="I44">
+        <v>19864</v>
+      </c>
+      <c r="J44">
+        <v>1201</v>
+      </c>
+      <c r="K44">
+        <v>116</v>
+      </c>
+      <c r="L44">
+        <v>186</v>
+      </c>
+      <c r="M44">
+        <v>497</v>
+      </c>
+      <c r="N44">
+        <v>0</v>
+      </c>
+      <c r="O44">
+        <v>0</v>
+      </c>
+      <c r="P44">
+        <f>SUM(C44:O44)</f>
+        <v>31802</v>
+      </c>
+      <c r="Q44" cm="1">
+        <f t="array" ref="Q44">SUM(ABS(C44:O44-C43:O43))</f>
+        <v>708</v>
+      </c>
+    </row>
+    <row r="45" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A45" s="1">
+        <v>44181</v>
+      </c>
+      <c r="B45">
+        <v>568</v>
+      </c>
+      <c r="C45">
+        <v>239</v>
+      </c>
+      <c r="D45">
+        <v>87</v>
+      </c>
+      <c r="E45">
+        <v>198</v>
+      </c>
+      <c r="F45">
+        <v>492</v>
+      </c>
+      <c r="G45">
+        <v>416</v>
+      </c>
+      <c r="H45">
+        <v>8524</v>
+      </c>
+      <c r="I45">
+        <v>19896</v>
+      </c>
+      <c r="J45">
+        <v>2460</v>
+      </c>
+      <c r="K45">
+        <v>116</v>
+      </c>
+      <c r="L45">
+        <v>186</v>
+      </c>
+      <c r="M45">
+        <v>497</v>
+      </c>
+      <c r="N45">
+        <v>0</v>
+      </c>
+      <c r="O45">
+        <v>0</v>
+      </c>
+      <c r="P45">
+        <f>SUM(C45:O45)</f>
+        <v>33111</v>
+      </c>
+      <c r="Q45" cm="1">
+        <f t="array" ref="Q45">SUM(ABS(C45:O45-C44:O44))</f>
+        <v>1309</v>
+      </c>
+    </row>
+    <row r="46" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A46" s="1">
+        <v>44182</v>
+      </c>
+      <c r="B46">
+        <v>568</v>
+      </c>
+      <c r="C46">
+        <v>239</v>
+      </c>
+      <c r="D46">
+        <v>87</v>
+      </c>
+      <c r="E46">
+        <v>198</v>
+      </c>
+      <c r="F46">
+        <v>492</v>
+      </c>
+      <c r="G46">
+        <v>416</v>
+      </c>
+      <c r="H46">
+        <v>8524</v>
+      </c>
+      <c r="I46">
+        <v>19896</v>
+      </c>
+      <c r="J46">
+        <v>3619</v>
+      </c>
+      <c r="K46">
+        <v>116</v>
+      </c>
+      <c r="L46">
+        <v>186</v>
+      </c>
+      <c r="M46">
+        <v>497</v>
+      </c>
+      <c r="N46">
+        <v>9</v>
+      </c>
+      <c r="O46">
+        <v>7</v>
+      </c>
+      <c r="P46">
+        <f>SUM(C46:O46)</f>
+        <v>34286</v>
+      </c>
+      <c r="Q46" cm="1">
+        <f t="array" ref="Q46">SUM(ABS(C46:O46-C45:O45))</f>
+        <v>1175</v>
+      </c>
+    </row>
+    <row r="47" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A47" s="1">
+        <v>44189</v>
+      </c>
+      <c r="B47">
+        <v>568</v>
+      </c>
+      <c r="C47">
+        <v>239</v>
+      </c>
+      <c r="D47">
+        <v>87</v>
+      </c>
+      <c r="E47">
+        <v>198</v>
+      </c>
+      <c r="F47">
+        <v>492</v>
+      </c>
+      <c r="G47">
+        <v>416</v>
+      </c>
+      <c r="H47">
+        <v>8524</v>
+      </c>
+      <c r="I47">
+        <v>19896</v>
+      </c>
+      <c r="J47">
+        <v>4447</v>
+      </c>
+      <c r="K47">
+        <v>116</v>
+      </c>
+      <c r="L47">
+        <v>186</v>
+      </c>
+      <c r="M47">
+        <v>497</v>
+      </c>
+      <c r="N47">
+        <v>9</v>
+      </c>
+      <c r="O47">
+        <v>7</v>
+      </c>
+      <c r="P47">
+        <f>SUM(C47:O47)</f>
+        <v>35114</v>
+      </c>
+      <c r="Q47" cm="1">
+        <f t="array" ref="Q47">SUM(ABS(C47:O47-C46:O46))</f>
+        <v>828</v>
+      </c>
+    </row>
+    <row r="48" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A48" s="1">
+        <v>44194</v>
+      </c>
+      <c r="B48">
+        <v>568</v>
+      </c>
+      <c r="C48">
+        <v>239</v>
+      </c>
+      <c r="D48">
+        <v>87</v>
+      </c>
+      <c r="E48">
+        <v>198</v>
+      </c>
+      <c r="F48">
+        <v>492</v>
+      </c>
+      <c r="G48">
+        <v>416</v>
+      </c>
+      <c r="H48">
+        <v>8524</v>
+      </c>
+      <c r="I48">
+        <v>19896</v>
+      </c>
+      <c r="J48">
+        <v>5634</v>
+      </c>
+      <c r="K48">
+        <v>116</v>
+      </c>
+      <c r="L48">
+        <v>186</v>
+      </c>
+      <c r="M48">
+        <v>497</v>
+      </c>
+      <c r="N48">
+        <v>9</v>
+      </c>
+      <c r="O48">
+        <v>7</v>
+      </c>
+      <c r="P48">
+        <f>SUM(C48:O48)</f>
+        <v>36301</v>
+      </c>
+      <c r="Q48" cm="1">
+        <f t="array" ref="Q48">SUM(ABS(C48:O48-C47:O47))</f>
+        <v>1187</v>
+      </c>
+    </row>
+    <row r="49" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A49" s="1">
+        <v>44195</v>
+      </c>
+      <c r="B49">
+        <v>568</v>
+      </c>
+      <c r="C49">
+        <v>239</v>
+      </c>
+      <c r="D49">
+        <v>87</v>
+      </c>
+      <c r="E49">
+        <v>229</v>
+      </c>
+      <c r="F49">
+        <v>492</v>
+      </c>
+      <c r="G49">
+        <v>416</v>
+      </c>
+      <c r="H49">
+        <v>8498</v>
+      </c>
+      <c r="I49">
+        <v>19876</v>
+      </c>
+      <c r="J49">
+        <v>5844</v>
+      </c>
+      <c r="K49">
+        <v>116</v>
+      </c>
+      <c r="L49">
+        <v>186</v>
+      </c>
+      <c r="M49">
+        <v>497</v>
+      </c>
+      <c r="N49">
+        <v>3559</v>
+      </c>
+      <c r="O49">
+        <v>7</v>
+      </c>
+      <c r="P49">
+        <f>SUM(C49:O49)</f>
+        <v>40046</v>
+      </c>
+      <c r="Q49" cm="1">
+        <f t="array" ref="Q49">SUM(ABS(C49:O49-C48:O48))</f>
+        <v>3837</v>
+      </c>
+    </row>
+    <row r="50" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A50" s="1">
+        <v>44197</v>
+      </c>
+      <c r="B50">
+        <v>631</v>
+      </c>
+      <c r="C50">
+        <v>239</v>
+      </c>
+      <c r="D50">
+        <v>87</v>
+      </c>
+      <c r="E50">
+        <v>229</v>
+      </c>
+      <c r="F50">
+        <v>492</v>
+      </c>
+      <c r="G50">
+        <v>416</v>
+      </c>
+      <c r="H50">
+        <v>8498</v>
+      </c>
+      <c r="I50">
+        <v>19876</v>
+      </c>
+      <c r="J50">
+        <v>5844</v>
+      </c>
+      <c r="K50">
+        <v>117</v>
+      </c>
+      <c r="L50">
+        <v>186</v>
+      </c>
+      <c r="M50">
+        <v>497</v>
+      </c>
+      <c r="N50">
+        <v>3559</v>
+      </c>
+      <c r="O50">
+        <v>1329</v>
+      </c>
+      <c r="P50">
+        <f>SUM(C50:O50)</f>
+        <v>41369</v>
+      </c>
+      <c r="Q50" cm="1">
+        <f t="array" ref="Q50">SUM(ABS(C50:O50-C49:O49))</f>
+        <v>1323</v>
+      </c>
+    </row>
+    <row r="51" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A51" s="1">
+        <v>44198</v>
+      </c>
+      <c r="B51">
+        <v>631</v>
+      </c>
+      <c r="C51">
+        <v>260</v>
+      </c>
+      <c r="D51">
+        <v>87</v>
+      </c>
+      <c r="E51">
+        <v>229</v>
+      </c>
+      <c r="F51">
+        <v>492</v>
+      </c>
+      <c r="G51">
+        <v>416</v>
+      </c>
+      <c r="H51">
+        <v>8550</v>
+      </c>
+      <c r="I51">
+        <v>19876</v>
+      </c>
+      <c r="J51">
+        <v>6122</v>
+      </c>
+      <c r="K51">
+        <v>117</v>
+      </c>
+      <c r="L51">
+        <v>186</v>
+      </c>
+      <c r="M51">
+        <v>496</v>
+      </c>
+      <c r="N51">
+        <v>3559</v>
+      </c>
+      <c r="O51">
+        <v>1329</v>
+      </c>
+      <c r="P51">
+        <f>SUM(C51:O51)</f>
+        <v>41719</v>
+      </c>
+      <c r="Q51">
+        <f>P51-P50</f>
+        <v>350</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Section 4.2: Interpreting the results
</commit_message>
<xml_diff>
--- a/thesis/progress.xlsx
+++ b/thesis/progress.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f7cf2c9d3dc7fdc6/Dissertation/thesis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="597" documentId="8_{8233B9E9-5E46-417E-8631-6A32EFB57DCE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{39BB63AA-9CDE-412E-AF89-1F0DA78EC461}"/>
+  <xr:revisionPtr revIDLastSave="616" documentId="8_{8233B9E9-5E46-417E-8631-6A32EFB57DCE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{33152130-83BD-4685-A6B9-C6F8D36C8A70}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" activeTab="1" xr2:uid="{90EBE93A-7825-427E-BCBE-4711C8076B47}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{90EBE93A-7825-427E-BCBE-4711C8076B47}"/>
   </bookViews>
   <sheets>
     <sheet name="dashboard" sheetId="3" r:id="rId1"/>
@@ -354,10 +354,10 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>writing!$A$2:$A$52</c:f>
+              <c:f>writing!$A$2:$A$53</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="51"/>
+                <c:ptCount val="52"/>
                 <c:pt idx="0">
                   <c:v>44130</c:v>
                 </c:pt>
@@ -510,16 +510,19 @@
                 </c:pt>
                 <c:pt idx="50">
                   <c:v>44210</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>44211</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>writing!$Q$2:$Q$52</c:f>
+              <c:f>writing!$Q$2:$Q$53</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="51"/>
+                <c:ptCount val="52"/>
                 <c:pt idx="0">
                   <c:v>1360</c:v>
                 </c:pt>
@@ -668,10 +671,13 @@
                   <c:v>1323</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>350</c:v>
+                  <c:v>352</c:v>
                 </c:pt>
                 <c:pt idx="50">
                   <c:v>336</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>976</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -783,10 +789,10 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>writing!$A$2:$A$52</c:f>
+              <c:f>writing!$A$2:$A$53</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="51"/>
+                <c:ptCount val="52"/>
                 <c:pt idx="0">
                   <c:v>44130</c:v>
                 </c:pt>
@@ -939,16 +945,19 @@
                 </c:pt>
                 <c:pt idx="50">
                   <c:v>44210</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>44211</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>writing!$P$2:$P$52</c:f>
+              <c:f>writing!$P$2:$P$53</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="51"/>
+                <c:ptCount val="52"/>
                 <c:pt idx="0">
                   <c:v>2614</c:v>
                 </c:pt>
@@ -1101,6 +1110,9 @@
                 </c:pt>
                 <c:pt idx="50">
                   <c:v>42055</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>43031</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2069,8 +2081,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{65BC4CFE-CBD1-4A0C-ACAB-8E0C8A33A81F}" name="Table1" displayName="Table1" ref="A1:Q52" totalsRowShown="0" headerRowDxfId="2">
-  <autoFilter ref="A1:Q52" xr:uid="{5C2EF26B-8F7C-40DC-90B6-805AC60B672A}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{65BC4CFE-CBD1-4A0C-ACAB-8E0C8A33A81F}" name="Table1" displayName="Table1" ref="A1:Q53" totalsRowShown="0" headerRowDxfId="2">
+  <autoFilter ref="A1:Q53" xr:uid="{5C2EF26B-8F7C-40DC-90B6-805AC60B672A}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:Q18">
     <sortCondition ref="A1:A18"/>
   </sortState>
@@ -2400,7 +2412,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CEB7023-1E9A-48AE-8417-31A8A140F136}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="P33" sqref="P33"/>
     </sheetView>
   </sheetViews>
@@ -2413,10 +2425,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F901F93A-6EBC-444E-BB8F-D0008D03E2AA}">
-  <dimension ref="A1:Q52"/>
+  <dimension ref="A1:Q53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F35" workbookViewId="0">
-      <selection activeCell="K52" sqref="K52"/>
+    <sheetView topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="A53" sqref="A53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -5235,9 +5247,9 @@
         <f t="shared" si="1"/>
         <v>41719</v>
       </c>
-      <c r="Q51">
-        <f>P51-P50</f>
-        <v>350</v>
+      <c r="Q51" cm="1">
+        <f t="array" ref="Q51">SUM(ABS(C51:O51-C50:O50))</f>
+        <v>352</v>
       </c>
     </row>
     <row r="52" spans="1:17" x14ac:dyDescent="0.45">
@@ -5290,9 +5302,64 @@
         <f>SUM(C52:O52)</f>
         <v>42055</v>
       </c>
-      <c r="Q52">
-        <f>P52-P51</f>
+      <c r="Q52" cm="1">
+        <f t="array" ref="Q52">SUM(ABS(C52:O52-C51:O51))</f>
         <v>336</v>
+      </c>
+    </row>
+    <row r="53" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="A53" s="1">
+        <v>44211</v>
+      </c>
+      <c r="B53">
+        <v>631</v>
+      </c>
+      <c r="C53">
+        <v>260</v>
+      </c>
+      <c r="D53">
+        <v>87</v>
+      </c>
+      <c r="E53">
+        <v>229</v>
+      </c>
+      <c r="F53">
+        <v>492</v>
+      </c>
+      <c r="G53">
+        <v>416</v>
+      </c>
+      <c r="H53">
+        <v>8587</v>
+      </c>
+      <c r="I53">
+        <v>19876</v>
+      </c>
+      <c r="J53">
+        <v>6417</v>
+      </c>
+      <c r="K53">
+        <v>1081</v>
+      </c>
+      <c r="L53">
+        <v>186</v>
+      </c>
+      <c r="M53">
+        <v>496</v>
+      </c>
+      <c r="N53">
+        <v>3575</v>
+      </c>
+      <c r="O53">
+        <v>1329</v>
+      </c>
+      <c r="P53">
+        <f>SUM(C53:O53)</f>
+        <v>43031</v>
+      </c>
+      <c r="Q53" cm="1">
+        <f t="array" ref="Q53">SUM(ABS(C53:O53-C52:O52))</f>
+        <v>976</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Section 4.3: Degree of lexical flexibility
</commit_message>
<xml_diff>
--- a/thesis/progress.xlsx
+++ b/thesis/progress.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f7cf2c9d3dc7fdc6/Dissertation/thesis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="618" documentId="8_{8233B9E9-5E46-417E-8631-6A32EFB57DCE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{885B32DF-3C59-40E5-B2D2-85E2E0B3BFC8}"/>
+  <xr:revisionPtr revIDLastSave="630" documentId="8_{8233B9E9-5E46-417E-8631-6A32EFB57DCE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{8A8185CA-6C84-4349-9F38-463CD39C4AE5}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{90EBE93A-7825-427E-BCBE-4711C8076B47}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="dashboard" sheetId="3" r:id="rId1"/>
     <sheet name="writing" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="191028" calcCompleted="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -354,10 +354,10 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>writing!$A$2:$A$53</c:f>
+              <c:f>writing!$A$2:$A$54</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="52"/>
+                <c:ptCount val="53"/>
                 <c:pt idx="0">
                   <c:v>44130</c:v>
                 </c:pt>
@@ -513,16 +513,19 @@
                 </c:pt>
                 <c:pt idx="51">
                   <c:v>44211</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>44212</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>writing!$Q$2:$Q$53</c:f>
+              <c:f>writing!$Q$2:$Q$54</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="52"/>
+                <c:ptCount val="53"/>
                 <c:pt idx="0">
                   <c:v>1360</c:v>
                 </c:pt>
@@ -678,6 +681,9 @@
                 </c:pt>
                 <c:pt idx="51">
                   <c:v>1134</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>1914</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -789,10 +795,10 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>writing!$A$2:$A$53</c:f>
+              <c:f>writing!$A$2:$A$54</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="52"/>
+                <c:ptCount val="53"/>
                 <c:pt idx="0">
                   <c:v>44130</c:v>
                 </c:pt>
@@ -948,16 +954,19 @@
                 </c:pt>
                 <c:pt idx="51">
                   <c:v>44211</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>44212</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>writing!$P$2:$P$53</c:f>
+              <c:f>writing!$P$2:$P$54</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="52"/>
+                <c:ptCount val="53"/>
                 <c:pt idx="0">
                   <c:v>2614</c:v>
                 </c:pt>
@@ -1113,6 +1122,9 @@
                 </c:pt>
                 <c:pt idx="51">
                   <c:v>43189</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>45103</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2081,8 +2093,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{65BC4CFE-CBD1-4A0C-ACAB-8E0C8A33A81F}" name="Table1" displayName="Table1" ref="A1:Q53" totalsRowShown="0" headerRowDxfId="2">
-  <autoFilter ref="A1:Q53" xr:uid="{5C2EF26B-8F7C-40DC-90B6-805AC60B672A}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{65BC4CFE-CBD1-4A0C-ACAB-8E0C8A33A81F}" name="Table1" displayName="Table1" ref="A1:Q54" totalsRowShown="0" headerRowDxfId="2">
+  <autoFilter ref="A1:Q54" xr:uid="{5C2EF26B-8F7C-40DC-90B6-805AC60B672A}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:Q18">
     <sortCondition ref="A1:A18"/>
   </sortState>
@@ -2425,10 +2437,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F901F93A-6EBC-444E-BB8F-D0008D03E2AA}">
-  <dimension ref="A1:Q53"/>
+  <dimension ref="A1:Q54"/>
   <sheetViews>
     <sheetView topLeftCell="F35" workbookViewId="0">
-      <selection activeCell="Q53" sqref="Q53"/>
+      <selection activeCell="L54" sqref="L54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -5362,6 +5374,61 @@
         <v>1134</v>
       </c>
     </row>
+    <row r="54" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="A54" s="1">
+        <v>44212</v>
+      </c>
+      <c r="B54">
+        <v>631</v>
+      </c>
+      <c r="C54">
+        <v>260</v>
+      </c>
+      <c r="D54">
+        <v>87</v>
+      </c>
+      <c r="E54">
+        <v>229</v>
+      </c>
+      <c r="F54">
+        <v>492</v>
+      </c>
+      <c r="G54">
+        <v>416</v>
+      </c>
+      <c r="H54">
+        <v>8725</v>
+      </c>
+      <c r="I54">
+        <v>19876</v>
+      </c>
+      <c r="J54">
+        <v>6562</v>
+      </c>
+      <c r="K54">
+        <v>2870</v>
+      </c>
+      <c r="L54">
+        <v>186</v>
+      </c>
+      <c r="M54">
+        <v>496</v>
+      </c>
+      <c r="N54">
+        <v>3575</v>
+      </c>
+      <c r="O54">
+        <v>1329</v>
+      </c>
+      <c r="P54">
+        <f>SUM(C54:O54)</f>
+        <v>45103</v>
+      </c>
+      <c r="Q54" cm="1">
+        <f t="array" ref="Q54">SUM(ABS(C54:O54-C53:O53))</f>
+        <v>1914</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>

<commit_message>
Ch. 2: BC edits (#932)
</commit_message>
<xml_diff>
--- a/thesis/progress.xlsx
+++ b/thesis/progress.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f7cf2c9d3dc7fdc6/Dissertation/thesis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="662" documentId="8_{8233B9E9-5E46-417E-8631-6A32EFB57DCE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{235BA3A1-0BCF-4956-9D4D-DB67BC5C4A71}"/>
+  <xr:revisionPtr revIDLastSave="669" documentId="8_{8233B9E9-5E46-417E-8631-6A32EFB57DCE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{61550F54-ED4F-4FA0-9D96-E26054E1C32F}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{90EBE93A-7825-427E-BCBE-4711C8076B47}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" activeTab="1" xr2:uid="{90EBE93A-7825-427E-BCBE-4711C8076B47}"/>
   </bookViews>
   <sheets>
     <sheet name="dashboard" sheetId="3" r:id="rId1"/>
@@ -354,10 +354,10 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>writing!$A$2:$A$58</c:f>
+              <c:f>writing!$A$2:$A$59</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="57"/>
+                <c:ptCount val="58"/>
                 <c:pt idx="0">
                   <c:v>44130</c:v>
                 </c:pt>
@@ -528,16 +528,19 @@
                 </c:pt>
                 <c:pt idx="56">
                   <c:v>44224</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>44225</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>writing!$Q$2:$Q$58</c:f>
+              <c:f>writing!$Q$2:$Q$59</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="57"/>
+                <c:ptCount val="58"/>
                 <c:pt idx="0">
                   <c:v>1360</c:v>
                 </c:pt>
@@ -708,6 +711,9 @@
                 </c:pt>
                 <c:pt idx="56">
                   <c:v>71</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>134</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -819,10 +825,10 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>writing!$A$2:$A$58</c:f>
+              <c:f>writing!$A$2:$A$59</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="57"/>
+                <c:ptCount val="58"/>
                 <c:pt idx="0">
                   <c:v>44130</c:v>
                 </c:pt>
@@ -993,16 +999,19 @@
                 </c:pt>
                 <c:pt idx="56">
                   <c:v>44224</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>44225</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>writing!$P$2:$P$58</c:f>
+              <c:f>writing!$P$2:$P$59</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="57"/>
+                <c:ptCount val="58"/>
                 <c:pt idx="0">
                   <c:v>2614</c:v>
                 </c:pt>
@@ -1173,6 +1182,9 @@
                 </c:pt>
                 <c:pt idx="56">
                   <c:v>50658</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>50588</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2141,8 +2153,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{65BC4CFE-CBD1-4A0C-ACAB-8E0C8A33A81F}" name="Table1" displayName="Table1" ref="A1:Q58" totalsRowShown="0" headerRowDxfId="2">
-  <autoFilter ref="A1:Q58" xr:uid="{5C2EF26B-8F7C-40DC-90B6-805AC60B672A}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{65BC4CFE-CBD1-4A0C-ACAB-8E0C8A33A81F}" name="Table1" displayName="Table1" ref="A1:Q59" totalsRowShown="0" headerRowDxfId="2">
+  <autoFilter ref="A1:Q59" xr:uid="{5C2EF26B-8F7C-40DC-90B6-805AC60B672A}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:Q18">
     <sortCondition ref="A1:A18"/>
   </sortState>
@@ -2472,7 +2484,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CEB7023-1E9A-48AE-8417-31A8A140F136}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="P33" sqref="P33"/>
     </sheetView>
   </sheetViews>
@@ -2485,10 +2497,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F901F93A-6EBC-444E-BB8F-D0008D03E2AA}">
-  <dimension ref="A1:Q58"/>
+  <dimension ref="A1:Q59"/>
   <sheetViews>
-    <sheetView topLeftCell="F35" workbookViewId="0">
-      <selection activeCell="L54" sqref="L54"/>
+    <sheetView tabSelected="1" topLeftCell="F35" workbookViewId="0">
+      <selection activeCell="N56" sqref="N56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -5697,6 +5709,61 @@
         <v>71</v>
       </c>
     </row>
+    <row r="59" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="A59" s="1">
+        <v>44225</v>
+      </c>
+      <c r="B59">
+        <v>631</v>
+      </c>
+      <c r="C59">
+        <v>260</v>
+      </c>
+      <c r="D59">
+        <v>87</v>
+      </c>
+      <c r="E59">
+        <v>229</v>
+      </c>
+      <c r="F59">
+        <v>492</v>
+      </c>
+      <c r="G59">
+        <v>416</v>
+      </c>
+      <c r="H59">
+        <v>8656</v>
+      </c>
+      <c r="I59">
+        <v>19908</v>
+      </c>
+      <c r="J59">
+        <v>6457</v>
+      </c>
+      <c r="K59">
+        <v>8497</v>
+      </c>
+      <c r="L59">
+        <v>186</v>
+      </c>
+      <c r="M59">
+        <v>496</v>
+      </c>
+      <c r="N59">
+        <v>3575</v>
+      </c>
+      <c r="O59">
+        <v>1329</v>
+      </c>
+      <c r="P59">
+        <f>SUM(C59:O59)</f>
+        <v>50588</v>
+      </c>
+      <c r="Q59" cm="1">
+        <f t="array" ref="Q59">SUM(ABS(C59:O59-C58:O58))</f>
+        <v>134</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>